<commit_message>
agregar parte de pago y formula al ER
</commit_message>
<xml_diff>
--- a/ER.xlsx
+++ b/ER.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\Archivos Importantes\Ucab\6. Sexto Semestre (6sem)\Sistemas de Bases de Datos I\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\GitHub\SBD1-Perfumeria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F115733D-3403-4F57-8D56-51D20E2DC74B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B019FB2-9788-4375-BA9F-E389D190E215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E58047A2-82F4-49D8-8F0D-4EA110376B37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Entidad" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
   <si>
     <t>Perfume</t>
   </si>
@@ -260,13 +261,109 @@
   </si>
   <si>
     <t>DET_ENVIO</t>
+  </si>
+  <si>
+    <t>Metodo de Pago</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cant_cuotas</t>
+  </si>
+  <si>
+    <t>modificador_precio</t>
+  </si>
+  <si>
+    <t>Pago en 2 cuotas de 50% con un interes o descuento de 5%</t>
+  </si>
+  <si>
+    <t>id_proveedor (mod log)</t>
+  </si>
+  <si>
+    <t>interes_descuento</t>
+  </si>
+  <si>
+    <t>det_metodo</t>
+  </si>
+  <si>
+    <t>mes_inicial</t>
+  </si>
+  <si>
+    <t>mes_final</t>
+  </si>
+  <si>
+    <t>porc</t>
+  </si>
+  <si>
+    <t>dia de pago</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>id_met</t>
+  </si>
+  <si>
+    <t>id_porc</t>
+  </si>
+  <si>
+    <t>id_dia</t>
+  </si>
+  <si>
+    <t>m_c</t>
+  </si>
+  <si>
+    <t>FK1</t>
+  </si>
+  <si>
+    <t>FK2</t>
+  </si>
+  <si>
+    <t>15 dias</t>
+  </si>
+  <si>
+    <t>coco</t>
+  </si>
+  <si>
+    <t>limon</t>
+  </si>
+  <si>
+    <t>3 limones</t>
+  </si>
+  <si>
+    <t>2 cocos</t>
+  </si>
+  <si>
+    <t>dia 0</t>
+  </si>
+  <si>
+    <t>5$</t>
+  </si>
+  <si>
+    <t>3$</t>
+  </si>
+  <si>
+    <t>9$</t>
+  </si>
+  <si>
+    <t>10$</t>
+  </si>
+  <si>
+    <t>19$</t>
+  </si>
+  <si>
+    <t>envio</t>
+  </si>
+  <si>
+    <t>24$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,8 +420,27 @@
       <color theme="7"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,8 +489,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -531,11 +659,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -570,6 +707,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,76 +752,93 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,377 +1169,377 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="I5" s="15" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="I5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="T5" s="15" t="s">
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="T5" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
     </row>
     <row r="6" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
     </row>
     <row r="7" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="I7" s="12" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="I7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14"/>
-      <c r="T7" s="17" t="s">
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="T7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
     </row>
     <row r="8" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="I8" s="12" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="I8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
-      <c r="T8" s="17" t="s">
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="T8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="T9" s="17" t="s">
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="T9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
     </row>
     <row r="10" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
     </row>
     <row r="12" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
       <c r="G12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="17"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="G13" s="6"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="G14" s="7"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
       <c r="G15" s="7"/>
-      <c r="U15" s="15" t="s">
+      <c r="U15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
     </row>
     <row r="16" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
       <c r="G16" s="7"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
     </row>
     <row r="17" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="U17" s="12" t="s">
+      <c r="U17" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="V17" s="13"/>
-      <c r="W17" s="14"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="26"/>
     </row>
     <row r="18" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
       <c r="G18" s="7"/>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="O18" s="15" t="s">
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="O18" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="U18" s="12" t="s">
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="U18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="V18" s="13"/>
-      <c r="W18" s="14"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="26"/>
     </row>
     <row r="19" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
       <c r="G19" s="7"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
       <c r="L19" s="3"/>
       <c r="M19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="N19" s="5"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
       <c r="V19" s="6"/>
     </row>
     <row r="20" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
       <c r="G20" s="7"/>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="O20" s="12" t="s">
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="O20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="14"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="26"/>
       <c r="V20" s="3"/>
     </row>
     <row r="21" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
       <c r="G21" s="7"/>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="O21" s="12" t="s">
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="O21" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="14"/>
-      <c r="U21" s="15" t="s">
+      <c r="P21" s="25"/>
+      <c r="Q21" s="26"/>
+      <c r="U21" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
     </row>
     <row r="22" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="9"/>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="I23" s="18" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="I23" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="U23" s="12" t="s">
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="U23" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="13"/>
-      <c r="W23" s="14"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="26"/>
     </row>
     <row r="24" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="I24" s="18" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+      <c r="I24" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="U24" s="12" t="s">
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="U24" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="V24" s="13"/>
-      <c r="W24" s="14"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="26"/>
     </row>
     <row r="25" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="I25" s="18" t="s">
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="26"/>
+      <c r="I25" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
       <c r="V26" s="3"/>
     </row>
     <row r="27" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="U27" s="15" t="s">
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+      <c r="U27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D28" s="6"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
     </row>
     <row r="29" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D29" s="7"/>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="U29" s="12" t="s">
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="U29" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="V29" s="13"/>
-      <c r="W29" s="14"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="26"/>
     </row>
     <row r="30" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D30" s="3"/>
@@ -1359,94 +1549,117 @@
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="U30" s="12" t="s">
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="U30" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="V30" s="13"/>
-      <c r="W30" s="14"/>
+      <c r="V30" s="25"/>
+      <c r="W30" s="26"/>
     </row>
     <row r="31" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="U31" s="12" t="s">
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="U31" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="V31" s="13"/>
-      <c r="W31" s="14"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="26"/>
     </row>
     <row r="32" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
       <c r="V32" s="6"/>
     </row>
     <row r="33" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I33" s="19" t="s">
+      <c r="I33" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
       <c r="V33" s="3"/>
     </row>
     <row r="34" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="U34" s="15" t="s">
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="U34" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="V34" s="15"/>
-      <c r="W34" s="15"/>
+      <c r="V34" s="23"/>
+      <c r="W34" s="23"/>
     </row>
     <row r="35" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="23"/>
+      <c r="W35" s="23"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="U36" s="12" t="s">
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="U36" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="V36" s="13"/>
-      <c r="W36" s="14"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="26"/>
     </row>
     <row r="37" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="U37" s="12" t="s">
+      <c r="U37" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="V37" s="13"/>
-      <c r="W37" s="14"/>
+      <c r="V37" s="25"/>
+      <c r="W37" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I5:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="U34:W35"/>
+    <mergeCell ref="U36:W36"/>
+    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="U21:W22"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="U27:W28"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="T5:W6"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="U15:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="I29:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="O18:Q19"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C26:E26"/>
@@ -1463,43 +1676,20 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="O18:Q19"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="T5:W6"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="U15:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="I29:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="U21:W22"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="U27:W28"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="U34:W35"/>
-    <mergeCell ref="U36:W36"/>
-    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1508,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A331C8E-6E8A-4DD1-B66D-75D29915EE06}">
-  <dimension ref="C4:AB54"/>
+  <dimension ref="C4:AB90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1527,220 +1717,220 @@
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="K5" s="22" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="K5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="O5" s="22" t="s">
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="O5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="S5" s="22" t="s">
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="S5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
       <c r="V5" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
       <c r="V6" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="S7" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
       <c r="V7" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="G9" s="20" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="G9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="K9" s="20" t="s">
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="K9" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="O9" s="22" t="s">
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="O9" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="S9" s="22" t="s">
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="S9" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
     </row>
     <row r="10" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
     </row>
     <row r="13" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="G13" s="20" t="s">
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="G13" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="K13" s="20" t="s">
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="K13" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="O13" s="20" t="s">
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="O13" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="S13" s="20" t="s">
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="S13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="G17" s="22" t="s">
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="G17" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="K17" s="22" t="s">
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="K17" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="O17" s="20" t="s">
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="O17" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="S17" s="20" t="s">
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="S17" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="T17" s="20"/>
-      <c r="U17" s="20"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20"/>
-      <c r="U18" s="20"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C19" s="11" t="s">
@@ -1748,69 +1938,69 @@
       </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="G21" s="22" t="s">
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="G21" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="K21" s="23" t="s">
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="K21" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="O21" s="20" t="s">
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="O21" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="S21" s="20" t="s">
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="S21" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="T21" s="20"/>
-      <c r="U21" s="20"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
     </row>
     <row r="25" spans="3:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="G25" s="22" t="s">
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="G25" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="27"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
@@ -1818,21 +2008,21 @@
       <c r="AA25" s="10"/>
     </row>
     <row r="26" spans="3:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10"/>
@@ -1847,7 +2037,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
-      <c r="R27" s="27"/>
+      <c r="R27" s="13"/>
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
@@ -1868,11 +2058,11 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
       <c r="U28" s="10"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
@@ -1886,16 +2076,16 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
@@ -1909,18 +2099,18 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
       <c r="N30" s="10"/>
-      <c r="O30" s="29" t="s">
+      <c r="O30" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
       <c r="W30" s="10"/>
@@ -1934,62 +2124,62 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
       <c r="U31" s="10"/>
       <c r="V31" s="10"/>
       <c r="W31" s="10"/>
-      <c r="X31" s="28"/>
-      <c r="Y31" s="26"/>
-      <c r="Z31" s="26"/>
-      <c r="AA31" s="26"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="12"/>
+      <c r="AA31" s="12"/>
     </row>
     <row r="32" spans="3:27" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
-      <c r="W32" s="26"/>
-      <c r="X32" s="26"/>
-      <c r="Y32" s="26"/>
-      <c r="Z32" s="26"/>
-      <c r="AA32" s="26"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="12"/>
     </row>
     <row r="33" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
       <c r="U33" s="10"/>
       <c r="V33" s="10"/>
       <c r="W33" s="10"/>
@@ -2003,16 +2193,16 @@
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
       <c r="U34" s="10"/>
       <c r="V34" s="10"/>
       <c r="W34" s="10"/>
@@ -2026,18 +2216,18 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="29" t="s">
+      <c r="O35" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
       <c r="U35" s="10"/>
       <c r="V35" s="10"/>
       <c r="W35" s="10"/>
@@ -2047,74 +2237,74 @@
       <c r="AA35" s="10"/>
     </row>
     <row r="36" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
       <c r="N36" s="10"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
       <c r="U36" s="10"/>
-      <c r="V36" s="27"/>
-      <c r="W36" s="26"/>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="25"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="33"/>
+      <c r="Y36" s="33"/>
       <c r="Z36" s="10"/>
       <c r="AA36" s="10"/>
     </row>
     <row r="37" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
       <c r="U37" s="10"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="25"/>
+      <c r="V37" s="12"/>
+      <c r="W37" s="12"/>
+      <c r="X37" s="33"/>
+      <c r="Y37" s="33"/>
       <c r="Z37" s="10"/>
       <c r="AA37" s="10"/>
     </row>
     <row r="38" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="26"/>
-      <c r="L38" s="26"/>
-      <c r="M38" s="26"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
       <c r="N38" s="10"/>
-      <c r="O38" s="29" t="s">
+      <c r="O38" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
       <c r="U38" s="10"/>
-      <c r="V38" s="27"/>
-      <c r="W38" s="26"/>
-      <c r="X38" s="26"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="12"/>
+      <c r="X38" s="12"/>
       <c r="Y38" s="10"/>
       <c r="Z38" s="10"/>
       <c r="AA38" s="10"/>
@@ -2124,70 +2314,70 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="29"/>
-      <c r="P39" s="29"/>
-      <c r="Q39" s="29"/>
-      <c r="R39" s="29"/>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
       <c r="U39" s="10"/>
-      <c r="V39" s="26"/>
-      <c r="W39" s="26"/>
-      <c r="X39" s="25"/>
-      <c r="Y39" s="25"/>
-      <c r="Z39" s="25"/>
-      <c r="AA39" s="25"/>
-      <c r="AB39" s="25"/>
+      <c r="V39" s="12"/>
+      <c r="W39" s="12"/>
+      <c r="X39" s="33"/>
+      <c r="Y39" s="33"/>
+      <c r="Z39" s="33"/>
+      <c r="AA39" s="33"/>
+      <c r="AB39" s="33"/>
     </row>
     <row r="40" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
       <c r="N40" s="10"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
       <c r="U40" s="10"/>
-      <c r="V40" s="27"/>
-      <c r="W40" s="26"/>
-      <c r="X40" s="25"/>
-      <c r="Y40" s="25"/>
-      <c r="Z40" s="25"/>
-      <c r="AA40" s="25"/>
-      <c r="AB40" s="25"/>
+      <c r="V40" s="13"/>
+      <c r="W40" s="12"/>
+      <c r="X40" s="33"/>
+      <c r="Y40" s="33"/>
+      <c r="Z40" s="33"/>
+      <c r="AA40" s="33"/>
+      <c r="AB40" s="33"/>
     </row>
     <row r="41" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
       <c r="N41" s="10"/>
-      <c r="O41" s="29" t="s">
+      <c r="O41" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
       <c r="U41" s="10"/>
-      <c r="V41" s="26"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="26"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="12"/>
       <c r="Y41" s="10"/>
       <c r="Z41" s="10"/>
       <c r="AA41" s="10"/>
@@ -2196,21 +2386,21 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
       <c r="N42" s="10"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="32"/>
+      <c r="R42" s="32"/>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
       <c r="U42" s="10"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="12"/>
       <c r="Y42" s="10"/>
       <c r="Z42" s="10"/>
       <c r="AA42" s="10"/>
@@ -2219,21 +2409,21 @@
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
       <c r="N43" s="10"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
       <c r="U43" s="10"/>
-      <c r="V43" s="26"/>
-      <c r="W43" s="26"/>
-      <c r="X43" s="26"/>
+      <c r="V43" s="12"/>
+      <c r="W43" s="12"/>
+      <c r="X43" s="12"/>
       <c r="Y43" s="10"/>
       <c r="Z43" s="10"/>
       <c r="AA43" s="10"/>
@@ -2247,21 +2437,21 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
-      <c r="O44" s="37"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="32"/>
+      <c r="Q44" s="32"/>
+      <c r="R44" s="32"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
       <c r="U44" s="10"/>
-      <c r="V44" s="27"/>
-      <c r="W44" s="26"/>
-      <c r="X44" s="29" t="s">
+      <c r="V44" s="13"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
+      <c r="Y44" s="32"/>
+      <c r="Z44" s="32"/>
+      <c r="AA44" s="32"/>
     </row>
     <row r="45" spans="7:28" x14ac:dyDescent="0.3">
       <c r="G45" s="10"/>
@@ -2272,19 +2462,19 @@
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
-      <c r="O45" s="29"/>
-      <c r="P45" s="29"/>
-      <c r="Q45" s="29"/>
-      <c r="R45" s="29"/>
-      <c r="S45" s="32"/>
-      <c r="T45" s="32"/>
-      <c r="U45" s="32"/>
-      <c r="V45" s="26"/>
-      <c r="W45" s="31"/>
-      <c r="X45" s="29"/>
-      <c r="Y45" s="29"/>
-      <c r="Z45" s="29"/>
-      <c r="AA45" s="29"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="32"/>
+      <c r="Y45" s="32"/>
+      <c r="Z45" s="32"/>
+      <c r="AA45" s="32"/>
     </row>
     <row r="46" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="10"/>
@@ -2295,201 +2485,490 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="29"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="32"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
-      <c r="U46" s="32"/>
-      <c r="V46" s="27"/>
-      <c r="W46" s="31"/>
-      <c r="X46" s="26"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="12"/>
       <c r="Y46" s="10"/>
       <c r="Z46" s="10"/>
       <c r="AA46" s="10"/>
     </row>
     <row r="47" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
-      <c r="Q47" s="38"/>
+      <c r="Q47" s="21"/>
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
-      <c r="U47" s="34"/>
-      <c r="V47" s="26"/>
-      <c r="W47" s="35"/>
-      <c r="X47" s="26"/>
+      <c r="U47" s="18"/>
+      <c r="V47" s="12"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="12"/>
       <c r="Y47" s="10"/>
       <c r="Z47" s="10"/>
       <c r="AA47" s="10"/>
     </row>
     <row r="48" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
-      <c r="Q48" s="32"/>
+      <c r="Q48" s="16"/>
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
-      <c r="U48" s="29" t="s">
+      <c r="U48" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="V48" s="29"/>
-      <c r="W48" s="29"/>
+      <c r="V48" s="32"/>
+      <c r="W48" s="32"/>
       <c r="X48" s="10"/>
       <c r="Y48" s="10"/>
       <c r="Z48" s="10"/>
       <c r="AA48" s="10"/>
     </row>
     <row r="49" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
-      <c r="Q49" s="32"/>
+      <c r="Q49" s="16"/>
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
-      <c r="U49" s="29"/>
-      <c r="V49" s="29"/>
-      <c r="W49" s="29"/>
+      <c r="U49" s="32"/>
+      <c r="V49" s="32"/>
+      <c r="W49" s="32"/>
       <c r="X49" s="10"/>
       <c r="Y49" s="10"/>
       <c r="Z49" s="10"/>
       <c r="AA49" s="10"/>
     </row>
     <row r="50" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
-      <c r="O50" s="29" t="s">
+      <c r="O50" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
+      <c r="P50" s="32"/>
+      <c r="Q50" s="32"/>
+      <c r="R50" s="32"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
-      <c r="U50" s="30" t="s">
+      <c r="U50" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="V50" s="30"/>
-      <c r="W50" s="30"/>
+      <c r="V50" s="34"/>
+      <c r="W50" s="34"/>
       <c r="X50" s="10"/>
       <c r="Y50" s="10"/>
       <c r="Z50" s="10"/>
       <c r="AA50" s="10"/>
     </row>
     <row r="51" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
-      <c r="O51" s="29"/>
-      <c r="P51" s="29"/>
-      <c r="Q51" s="29"/>
-      <c r="R51" s="29"/>
-      <c r="U51" s="30"/>
-      <c r="V51" s="30"/>
-      <c r="W51" s="30"/>
+      <c r="O51" s="32"/>
+      <c r="P51" s="32"/>
+      <c r="Q51" s="32"/>
+      <c r="R51" s="32"/>
+      <c r="U51" s="34"/>
+      <c r="V51" s="34"/>
+      <c r="W51" s="34"/>
     </row>
     <row r="52" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
-      <c r="U52" s="24" t="s">
+      <c r="U52" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="V52" s="24"/>
-      <c r="W52" s="24"/>
+      <c r="V52" s="30"/>
+      <c r="W52" s="30"/>
     </row>
     <row r="53" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
-      <c r="U53" s="24"/>
-      <c r="V53" s="24"/>
-      <c r="W53" s="24"/>
+      <c r="U53" s="30"/>
+      <c r="V53" s="30"/>
+      <c r="W53" s="30"/>
     </row>
     <row r="54" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
     </row>
+    <row r="63" spans="7:27" x14ac:dyDescent="0.3">
+      <c r="V63" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="W63" s="32"/>
+      <c r="X63" s="32"/>
+      <c r="Y63" s="32"/>
+    </row>
+    <row r="64" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O64" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="P64" s="32"/>
+      <c r="Q64" s="32"/>
+      <c r="R64" s="32"/>
+      <c r="V64" s="32"/>
+      <c r="W64" s="32"/>
+      <c r="X64" s="32"/>
+      <c r="Y64" s="32"/>
+    </row>
+    <row r="65" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G65" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="32"/>
+      <c r="P65" s="32"/>
+      <c r="Q65" s="32"/>
+      <c r="R65" s="32"/>
+      <c r="V65" s="32"/>
+      <c r="W65" s="32"/>
+      <c r="X65" s="32"/>
+      <c r="Y65" s="32"/>
+    </row>
+    <row r="66" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="32"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="P66" s="34"/>
+      <c r="Q66" s="34"/>
+      <c r="R66" s="34"/>
+      <c r="V66" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="W66" s="32"/>
+      <c r="X66" s="32"/>
+      <c r="Y66" s="32"/>
+    </row>
+    <row r="67" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="34"/>
+      <c r="P67" s="34"/>
+      <c r="Q67" s="34"/>
+      <c r="R67" s="34"/>
+      <c r="V67" s="32"/>
+      <c r="W67" s="32"/>
+      <c r="X67" s="32"/>
+      <c r="Y67" s="32"/>
+    </row>
+    <row r="68" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O68" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="P68" s="30"/>
+      <c r="Q68" s="30"/>
+      <c r="R68" s="30"/>
+      <c r="V68" s="32"/>
+      <c r="W68" s="32"/>
+      <c r="X68" s="32"/>
+      <c r="Y68" s="32"/>
+    </row>
+    <row r="69" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O69" s="30"/>
+      <c r="P69" s="30"/>
+      <c r="Q69" s="30"/>
+      <c r="R69" s="30"/>
+      <c r="V69" s="32"/>
+      <c r="W69" s="32"/>
+      <c r="X69" s="32"/>
+      <c r="Y69" s="32"/>
+    </row>
+    <row r="70" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O70" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="P70" s="41"/>
+      <c r="Q70" s="41"/>
+      <c r="R70" s="41"/>
+      <c r="S70" s="41"/>
+      <c r="V70" s="32"/>
+      <c r="W70" s="32"/>
+      <c r="X70" s="32"/>
+      <c r="Y70" s="32"/>
+    </row>
+    <row r="71" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O71" s="41"/>
+      <c r="P71" s="41"/>
+      <c r="Q71" s="41"/>
+      <c r="R71" s="41"/>
+      <c r="S71" s="41"/>
+      <c r="V71" s="32"/>
+      <c r="W71" s="32"/>
+      <c r="X71" s="32"/>
+      <c r="Y71" s="32"/>
+    </row>
+    <row r="72" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="V72" s="31"/>
+      <c r="W72" s="32"/>
+      <c r="X72" s="32"/>
+      <c r="Y72" s="32"/>
+    </row>
+    <row r="73" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="K73" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="V73" s="32"/>
+      <c r="W73" s="32"/>
+      <c r="X73" s="32"/>
+      <c r="Y73" s="32"/>
+    </row>
+    <row r="74" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="V74" s="32"/>
+      <c r="W74" s="32"/>
+      <c r="X74" s="32"/>
+      <c r="Y74" s="32"/>
+    </row>
+    <row r="79" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="V79" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="W79" s="32"/>
+      <c r="X79" s="32"/>
+      <c r="Y79" s="32"/>
+    </row>
+    <row r="80" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="O80" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P80" s="32"/>
+      <c r="Q80" s="32"/>
+      <c r="R80" s="32"/>
+      <c r="V80" s="32"/>
+      <c r="W80" s="32"/>
+      <c r="X80" s="32"/>
+      <c r="Y80" s="32"/>
+    </row>
+    <row r="81" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="G81" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H81" s="32"/>
+      <c r="I81" s="32"/>
+      <c r="J81" s="32"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="32"/>
+      <c r="P81" s="32"/>
+      <c r="Q81" s="32"/>
+      <c r="R81" s="32"/>
+      <c r="V81" s="32"/>
+      <c r="W81" s="32"/>
+      <c r="X81" s="32"/>
+      <c r="Y81" s="32"/>
+    </row>
+    <row r="82" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="32"/>
+      <c r="J82" s="32"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="18"/>
+      <c r="O82" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="P82" s="34"/>
+      <c r="Q82" s="34"/>
+      <c r="R82" s="34"/>
+      <c r="S82" s="40"/>
+      <c r="V82" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="W82" s="32"/>
+      <c r="X82" s="32"/>
+      <c r="Y82" s="32"/>
+    </row>
+    <row r="83" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="G83" s="32"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="32"/>
+      <c r="J83" s="32"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="34"/>
+      <c r="P83" s="34"/>
+      <c r="Q83" s="34"/>
+      <c r="R83" s="34"/>
+      <c r="S83" s="40"/>
+      <c r="T83" s="39"/>
+      <c r="U83" s="39"/>
+      <c r="V83" s="32"/>
+      <c r="W83" s="32"/>
+      <c r="X83" s="32"/>
+      <c r="Y83" s="32"/>
+    </row>
+    <row r="84" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="O84" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="P84" s="30"/>
+      <c r="Q84" s="30"/>
+      <c r="R84" s="30"/>
+      <c r="S84" s="40"/>
+      <c r="V84" s="32"/>
+      <c r="W84" s="32"/>
+      <c r="X84" s="32"/>
+      <c r="Y84" s="32"/>
+    </row>
+    <row r="85" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="O85" s="30"/>
+      <c r="P85" s="30"/>
+      <c r="Q85" s="30"/>
+      <c r="R85" s="30"/>
+      <c r="V85" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="W85" s="32"/>
+      <c r="X85" s="32"/>
+      <c r="Y85" s="32"/>
+    </row>
+    <row r="86" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O86" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="P86" s="30"/>
+      <c r="Q86" s="30"/>
+      <c r="R86" s="30"/>
+      <c r="S86" s="42"/>
+      <c r="V86" s="32"/>
+      <c r="W86" s="32"/>
+      <c r="X86" s="32"/>
+      <c r="Y86" s="32"/>
+    </row>
+    <row r="87" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O87" s="30"/>
+      <c r="P87" s="30"/>
+      <c r="Q87" s="30"/>
+      <c r="R87" s="30"/>
+      <c r="S87" s="42"/>
+      <c r="V87" s="32"/>
+      <c r="W87" s="32"/>
+      <c r="X87" s="32"/>
+      <c r="Y87" s="32"/>
+    </row>
+    <row r="88" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="V88" s="32"/>
+      <c r="W88" s="32"/>
+      <c r="X88" s="32"/>
+      <c r="Y88" s="32"/>
+    </row>
+    <row r="89" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="K89" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="V89" s="32"/>
+      <c r="W89" s="32"/>
+      <c r="X89" s="32"/>
+      <c r="Y89" s="32"/>
+    </row>
+    <row r="90" spans="7:25" x14ac:dyDescent="0.3">
+      <c r="V90" s="32"/>
+      <c r="W90" s="32"/>
+      <c r="X90" s="32"/>
+      <c r="Y90" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="U52:W53"/>
-    <mergeCell ref="O44:R46"/>
-    <mergeCell ref="X36:Y37"/>
-    <mergeCell ref="X39:AB40"/>
-    <mergeCell ref="O50:R51"/>
-    <mergeCell ref="X44:AA45"/>
-    <mergeCell ref="U48:W49"/>
-    <mergeCell ref="U50:W51"/>
-    <mergeCell ref="G36:J38"/>
-    <mergeCell ref="O30:R31"/>
-    <mergeCell ref="O35:R37"/>
-    <mergeCell ref="O38:R40"/>
-    <mergeCell ref="O41:R43"/>
-    <mergeCell ref="S5:U6"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="K9:M10"/>
-    <mergeCell ref="O9:Q10"/>
-    <mergeCell ref="S9:U10"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="K5:M6"/>
-    <mergeCell ref="O5:Q6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="C13:E14"/>
-    <mergeCell ref="G13:I14"/>
-    <mergeCell ref="K13:M14"/>
+  <mergeCells count="62">
+    <mergeCell ref="V88:Y90"/>
+    <mergeCell ref="O86:R87"/>
+    <mergeCell ref="V79:Y81"/>
+    <mergeCell ref="O80:R81"/>
+    <mergeCell ref="G81:J83"/>
+    <mergeCell ref="O82:R83"/>
+    <mergeCell ref="V82:Y84"/>
+    <mergeCell ref="O84:R85"/>
+    <mergeCell ref="V85:Y87"/>
+    <mergeCell ref="G65:J67"/>
+    <mergeCell ref="V63:Y65"/>
+    <mergeCell ref="V66:Y68"/>
+    <mergeCell ref="V69:Y71"/>
+    <mergeCell ref="V72:Y74"/>
+    <mergeCell ref="O64:R65"/>
+    <mergeCell ref="O66:R67"/>
+    <mergeCell ref="O68:R69"/>
+    <mergeCell ref="O70:S71"/>
     <mergeCell ref="C25:E26"/>
     <mergeCell ref="G25:I26"/>
     <mergeCell ref="O13:Q14"/>
@@ -2504,8 +2983,295 @@
     <mergeCell ref="K17:M18"/>
     <mergeCell ref="O17:Q18"/>
     <mergeCell ref="S17:U18"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="G13:I14"/>
+    <mergeCell ref="K13:M14"/>
+    <mergeCell ref="S5:U6"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="K9:M10"/>
+    <mergeCell ref="O9:Q10"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="K5:M6"/>
+    <mergeCell ref="O5:Q6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="G36:J38"/>
+    <mergeCell ref="O30:R31"/>
+    <mergeCell ref="O35:R37"/>
+    <mergeCell ref="O38:R40"/>
+    <mergeCell ref="O41:R43"/>
+    <mergeCell ref="U52:W53"/>
+    <mergeCell ref="O44:R46"/>
+    <mergeCell ref="X36:Y37"/>
+    <mergeCell ref="X39:AB40"/>
+    <mergeCell ref="O50:R51"/>
+    <mergeCell ref="X44:AA45"/>
+    <mergeCell ref="U48:W49"/>
+    <mergeCell ref="U50:W51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E37153-5D58-49F3-A7E8-18914BA10F81}">
+  <dimension ref="C2:T16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="33.6" x14ac:dyDescent="0.65"/>
+  <cols>
+    <col min="1" max="10" width="8.88671875" style="43"/>
+    <col min="11" max="11" width="15" style="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="C2" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="C3" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="C4" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="53"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="54"/>
+      <c r="P4" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="C5" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="52"/>
+      <c r="G5" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="52"/>
+      <c r="K5" s="44"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="K6" s="44"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="50">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46">
+        <v>0</v>
+      </c>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="K7" s="44"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="50">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46">
+        <v>0</v>
+      </c>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="H8" s="43">
+        <v>100</v>
+      </c>
+      <c r="J8" s="43">
+        <v>0</v>
+      </c>
+      <c r="K8" s="44"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="50">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46">
+        <v>15</v>
+      </c>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="H9" s="43">
+        <v>25</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="50">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46">
+        <v>30</v>
+      </c>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="50">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46">
+        <v>45</v>
+      </c>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="G12" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="L12" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="P12" s="43">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="G13" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="L14" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="L15" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" s="43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.65">
+      <c r="L16" s="43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agregar cosas del ER
</commit_message>
<xml_diff>
--- a/ER.xlsx
+++ b/ER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\GitHub\SBD1-Perfumeria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B019FB2-9788-4375-BA9F-E389D190E215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A8E1FD-9363-469D-B39B-189B7BE2874E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E58047A2-82F4-49D8-8F0D-4EA110376B37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E58047A2-82F4-49D8-8F0D-4EA110376B37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
   <si>
     <t>Perfume</t>
   </si>
@@ -357,13 +357,79 @@
   </si>
   <si>
     <t>24$</t>
+  </si>
+  <si>
+    <t>id_crit</t>
+  </si>
+  <si>
+    <t>id_form</t>
+  </si>
+  <si>
+    <t>id_Region</t>
+  </si>
+  <si>
+    <t>id_pago</t>
+  </si>
+  <si>
+    <t>id_envio</t>
+  </si>
+  <si>
+    <t>id_cump</t>
+  </si>
+  <si>
+    <t>puntos</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>CASO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>PK1</t>
+  </si>
+  <si>
+    <t>FK3</t>
+  </si>
+  <si>
+    <t>FK4</t>
+  </si>
+  <si>
+    <t>FK5</t>
+  </si>
+  <si>
+    <t>peso</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>VALORACION</t>
+  </si>
+  <si>
+    <t>80/100</t>
+  </si>
+  <si>
+    <t>los puntos suman 100 por criterio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,8 +505,20 @@
       <color theme="5"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,8 +579,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -668,11 +758,183 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -737,110 +999,196 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1157,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075D56C9-9013-44E8-86C7-ACC885266A1C}">
   <dimension ref="C5:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -1169,377 +1517,377 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="I5" s="23" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="I5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="T5" s="23" t="s">
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="T5" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
     </row>
     <row r="6" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
     </row>
     <row r="7" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="I7" s="24" t="s">
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="I7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-      <c r="T7" s="28" t="s">
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+      <c r="T7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
     </row>
     <row r="8" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="I8" s="24" t="s">
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="I8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
-      <c r="T8" s="28" t="s">
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+      <c r="T8" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="U8" s="28"/>
-      <c r="V8" s="28"/>
-      <c r="W8" s="28"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-      <c r="T9" s="28" t="s">
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
+      <c r="T9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
     </row>
     <row r="10" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="28"/>
-      <c r="W11" s="28"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
     </row>
     <row r="12" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
       <c r="G12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
       <c r="G13" s="6"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
       <c r="G14" s="7"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
       <c r="G15" s="7"/>
-      <c r="U15" s="23" t="s">
+      <c r="U15" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
     </row>
     <row r="16" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
       <c r="G16" s="7"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
     </row>
     <row r="17" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="U17" s="24" t="s">
+      <c r="U17" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="29"/>
     </row>
     <row r="18" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
       <c r="G18" s="7"/>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="O18" s="23" t="s">
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="O18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="U18" s="24" t="s">
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="U18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="V18" s="25"/>
-      <c r="W18" s="26"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="29"/>
     </row>
     <row r="19" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
       <c r="G19" s="7"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
       <c r="L19" s="3"/>
       <c r="M19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="N19" s="5"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
       <c r="V19" s="6"/>
     </row>
     <row r="20" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
       <c r="G20" s="7"/>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="O20" s="24" t="s">
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="O20" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="29"/>
       <c r="V20" s="3"/>
     </row>
     <row r="21" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
       <c r="G21" s="7"/>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="O21" s="24" t="s">
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="O21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="26"/>
-      <c r="U21" s="23" t="s">
+      <c r="P21" s="28"/>
+      <c r="Q21" s="29"/>
+      <c r="U21" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
     </row>
     <row r="22" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="9"/>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
-      <c r="I23" s="22" t="s">
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="I23" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="U23" s="24" t="s">
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="U23" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="25"/>
-      <c r="W23" s="26"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="29"/>
     </row>
     <row r="24" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="I24" s="22" t="s">
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+      <c r="I24" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="U24" s="24" t="s">
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="U24" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="29"/>
     </row>
     <row r="25" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
-      <c r="I25" s="22" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="I25" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
       <c r="V26" s="3"/>
     </row>
     <row r="27" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26"/>
-      <c r="U27" s="23" t="s">
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="U27" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D28" s="6"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
     </row>
     <row r="29" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D29" s="7"/>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="U29" s="24" t="s">
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="U29" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="V29" s="25"/>
-      <c r="W29" s="26"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="29"/>
     </row>
     <row r="30" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D30" s="3"/>
@@ -1549,90 +1897,121 @@
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="U30" s="24" t="s">
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="U30" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="V30" s="25"/>
-      <c r="W30" s="26"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="29"/>
     </row>
     <row r="31" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="U31" s="24" t="s">
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="U31" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="V31" s="25"/>
-      <c r="W31" s="26"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="29"/>
     </row>
     <row r="32" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="I32" s="29" t="s">
+      <c r="I32" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
       <c r="V32" s="6"/>
     </row>
     <row r="33" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I33" s="29" t="s">
+      <c r="I33" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
       <c r="V33" s="3"/>
     </row>
     <row r="34" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="U34" s="23" t="s">
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="U34" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="V34" s="23"/>
-      <c r="W34" s="23"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
     </row>
     <row r="35" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="23"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="U36" s="24" t="s">
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="U36" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="V36" s="25"/>
-      <c r="W36" s="26"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="29"/>
     </row>
     <row r="37" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="U37" s="24" t="s">
+      <c r="U37" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="V37" s="25"/>
-      <c r="W37" s="26"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="U34:W35"/>
-    <mergeCell ref="U36:W36"/>
-    <mergeCell ref="U37:W37"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="U21:W22"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="U27:W28"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="C18:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="I18:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="O18:Q19"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
     <mergeCell ref="U29:W29"/>
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="T5:W6"/>
@@ -1649,47 +2028,16 @@
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="I33:K33"/>
     <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="O18:Q19"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="C18:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="I18:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I5:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="U21:W22"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="U27:W28"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="U34:W35"/>
+    <mergeCell ref="U36:W36"/>
+    <mergeCell ref="U37:W37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1700,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A331C8E-6E8A-4DD1-B66D-75D29915EE06}">
   <dimension ref="C4:AB90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="F29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N46" sqref="M46:N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1717,220 +2065,220 @@
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="K5" s="35" t="s">
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="K5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="O5" s="35" t="s">
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="O5" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="S5" s="35" t="s">
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="S5" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
       <c r="V5" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
       <c r="V6" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="37" t="s">
+      <c r="S7" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
       <c r="V7" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="G9" s="36" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="G9" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="K9" s="36" t="s">
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="K9" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="O9" s="35" t="s">
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="O9" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="S9" s="35" t="s">
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="S9" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
     </row>
     <row r="10" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="13" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="G13" s="57" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="G13" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="K13" s="36" t="s">
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="K13" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="O13" s="36" t="s">
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="O13" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="S13" s="36" t="s">
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="S13" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="G17" s="35" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="G17" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="K17" s="35" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="K17" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="O17" s="36" t="s">
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="O17" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="S17" s="36" t="s">
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="S17" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C19" s="11" t="s">
@@ -1938,60 +2286,60 @@
       </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="G21" s="35" t="s">
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="G21" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="K21" s="38" t="s">
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="K21" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="O21" s="36" t="s">
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="O21" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="S21" s="36" t="s">
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="S21" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
     </row>
     <row r="25" spans="3:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="G25" s="35" t="s">
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="G25" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
@@ -2008,12 +2356,12 @@
       <c r="AA25" s="10"/>
     </row>
     <row r="26" spans="3:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
@@ -2103,12 +2451,12 @@
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
       <c r="N30" s="10"/>
-      <c r="O30" s="32" t="s">
+      <c r="O30" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
-      <c r="R30" s="32"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="10"/>
@@ -2128,10 +2476,10 @@
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="32"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
       <c r="U31" s="10"/>
@@ -2217,15 +2565,15 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="13"/>
-      <c r="L35" s="12"/>
+      <c r="L35" s="82"/>
       <c r="M35" s="12"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="32" t="s">
+      <c r="O35" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="32"/>
-      <c r="R35" s="32"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="10"/>
@@ -2237,68 +2585,68 @@
       <c r="AA35" s="10"/>
     </row>
     <row r="36" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="32" t="s">
+      <c r="G36" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
+      <c r="L36" s="82"/>
       <c r="M36" s="12"/>
       <c r="N36" s="10"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
       <c r="S36" s="13"/>
       <c r="T36" s="13"/>
       <c r="U36" s="10"/>
       <c r="V36" s="13"/>
       <c r="W36" s="12"/>
-      <c r="X36" s="33"/>
-      <c r="Y36" s="33"/>
+      <c r="X36" s="45"/>
+      <c r="Y36" s="45"/>
       <c r="Z36" s="10"/>
       <c r="AA36" s="10"/>
     </row>
     <row r="37" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
       <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
+      <c r="L37" s="82"/>
       <c r="M37" s="15"/>
       <c r="N37" s="18"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="32"/>
-      <c r="R37" s="32"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
       <c r="U37" s="10"/>
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
-      <c r="X37" s="33"/>
-      <c r="Y37" s="33"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
       <c r="Z37" s="10"/>
       <c r="AA37" s="10"/>
     </row>
     <row r="38" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="L38" s="82"/>
       <c r="M38" s="12"/>
       <c r="N38" s="10"/>
-      <c r="O38" s="32" t="s">
+      <c r="O38" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="32"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
       <c r="S38" s="13"/>
       <c r="T38" s="13"/>
       <c r="U38" s="10"/>
@@ -2315,23 +2663,23 @@
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="L39" s="82"/>
       <c r="M39" s="12"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
-      <c r="R39" s="32"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
       <c r="U39" s="10"/>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
-      <c r="X39" s="33"/>
-      <c r="Y39" s="33"/>
-      <c r="Z39" s="33"/>
-      <c r="AA39" s="33"/>
-      <c r="AB39" s="33"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
     </row>
     <row r="40" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G40" s="10"/>
@@ -2342,20 +2690,20 @@
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
       <c r="N40" s="10"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="R40" s="32"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
       <c r="U40" s="10"/>
       <c r="V40" s="13"/>
       <c r="W40" s="12"/>
-      <c r="X40" s="33"/>
-      <c r="Y40" s="33"/>
-      <c r="Z40" s="33"/>
-      <c r="AA40" s="33"/>
-      <c r="AB40" s="33"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
+      <c r="AB40" s="45"/>
     </row>
     <row r="41" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="10"/>
@@ -2366,12 +2714,12 @@
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
       <c r="N41" s="10"/>
-      <c r="O41" s="32" t="s">
+      <c r="O41" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
       <c r="U41" s="10"/>
@@ -2391,10 +2739,10 @@
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
       <c r="N42" s="10"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="32"/>
-      <c r="R42" s="32"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
       <c r="U42" s="10"/>
@@ -2414,10 +2762,10 @@
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
       <c r="N43" s="10"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="32"/>
-      <c r="R43" s="32"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
       <c r="U43" s="10"/>
@@ -2429,7 +2777,7 @@
       <c r="AA43" s="10"/>
     </row>
     <row r="44" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G44" s="10"/>
+      <c r="G44" s="83"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
@@ -2437,24 +2785,26 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
-      <c r="O44" s="31"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="32"/>
-      <c r="R44" s="32"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="35"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
       <c r="U44" s="10"/>
       <c r="V44" s="13"/>
       <c r="W44" s="12"/>
-      <c r="X44" s="32" t="s">
+      <c r="X44" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="Y44" s="32"/>
-      <c r="Z44" s="32"/>
-      <c r="AA44" s="32"/>
+      <c r="Y44" s="35"/>
+      <c r="Z44" s="35"/>
+      <c r="AA44" s="35"/>
     </row>
     <row r="45" spans="7:28" x14ac:dyDescent="0.3">
-      <c r="G45" s="10"/>
+      <c r="G45" s="83" t="s">
+        <v>123</v>
+      </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
@@ -2462,33 +2812,35 @@
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="32"/>
-      <c r="R45" s="32"/>
+      <c r="O45" s="35"/>
+      <c r="P45" s="35"/>
+      <c r="Q45" s="35"/>
+      <c r="R45" s="35"/>
       <c r="S45" s="16"/>
       <c r="T45" s="16"/>
       <c r="U45" s="16"/>
       <c r="V45" s="12"/>
       <c r="W45" s="15"/>
-      <c r="X45" s="32"/>
-      <c r="Y45" s="32"/>
-      <c r="Z45" s="32"/>
-      <c r="AA45" s="32"/>
+      <c r="X45" s="35"/>
+      <c r="Y45" s="35"/>
+      <c r="Z45" s="35"/>
+      <c r="AA45" s="35"/>
     </row>
     <row r="46" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
+      <c r="G46" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="83"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="32"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="35"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
       <c r="U46" s="16"/>
@@ -2500,12 +2852,14 @@
       <c r="AA46" s="10"/>
     </row>
     <row r="47" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G47" s="13"/>
+      <c r="G47" s="86" t="s">
+        <v>125</v>
+      </c>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
+      <c r="L47" s="83"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
@@ -2523,12 +2877,14 @@
       <c r="AA47" s="10"/>
     </row>
     <row r="48" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="13"/>
+      <c r="G48" s="85" t="s">
+        <v>126</v>
+      </c>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
+      <c r="L48" s="83"/>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
@@ -2537,23 +2893,23 @@
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
-      <c r="U48" s="32" t="s">
+      <c r="U48" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="V48" s="32"/>
-      <c r="W48" s="32"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="35"/>
       <c r="X48" s="10"/>
       <c r="Y48" s="10"/>
       <c r="Z48" s="10"/>
       <c r="AA48" s="10"/>
     </row>
     <row r="49" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G49" s="13"/>
+      <c r="G49" s="84"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
+      <c r="L49" s="83"/>
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
@@ -2562,9 +2918,9 @@
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
-      <c r="U49" s="32"/>
-      <c r="V49" s="32"/>
-      <c r="W49" s="32"/>
+      <c r="U49" s="35"/>
+      <c r="V49" s="35"/>
+      <c r="W49" s="35"/>
       <c r="X49" s="10"/>
       <c r="Y49" s="10"/>
       <c r="Z49" s="10"/>
@@ -2576,22 +2932,22 @@
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
       <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="32" t="s">
+      <c r="L50" s="83"/>
+      <c r="M50" s="83"/>
+      <c r="N50" s="83"/>
+      <c r="O50" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="32"/>
-      <c r="R50" s="32"/>
+      <c r="P50" s="35"/>
+      <c r="Q50" s="35"/>
+      <c r="R50" s="35"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
-      <c r="U50" s="34" t="s">
+      <c r="U50" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="V50" s="34"/>
-      <c r="W50" s="34"/>
+      <c r="V50" s="38"/>
+      <c r="W50" s="38"/>
       <c r="X50" s="10"/>
       <c r="Y50" s="10"/>
       <c r="Z50" s="10"/>
@@ -2605,13 +2961,13 @@
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="32"/>
-      <c r="U51" s="34"/>
-      <c r="V51" s="34"/>
-      <c r="W51" s="34"/>
+      <c r="O51" s="35"/>
+      <c r="P51" s="35"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="35"/>
+      <c r="U51" s="38"/>
+      <c r="V51" s="38"/>
+      <c r="W51" s="38"/>
     </row>
     <row r="52" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G52" s="13"/>
@@ -2621,11 +2977,11 @@
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
-      <c r="U52" s="30" t="s">
+      <c r="U52" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="V52" s="30"/>
-      <c r="W52" s="30"/>
+      <c r="V52" s="37"/>
+      <c r="W52" s="37"/>
     </row>
     <row r="53" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G53" s="13"/>
@@ -2635,9 +2991,9 @@
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
-      <c r="U53" s="30"/>
-      <c r="V53" s="30"/>
-      <c r="W53" s="30"/>
+      <c r="U53" s="37"/>
+      <c r="V53" s="37"/>
+      <c r="W53" s="37"/>
     </row>
     <row r="54" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G54" s="13"/>
@@ -2649,326 +3005,338 @@
       <c r="M54" s="10"/>
     </row>
     <row r="63" spans="7:27" x14ac:dyDescent="0.3">
-      <c r="V63" s="32" t="s">
+      <c r="V63" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="W63" s="32"/>
-      <c r="X63" s="32"/>
-      <c r="Y63" s="32"/>
+      <c r="W63" s="35"/>
+      <c r="X63" s="35"/>
+      <c r="Y63" s="35"/>
     </row>
     <row r="64" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O64" s="32" t="s">
+      <c r="O64" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="P64" s="32"/>
-      <c r="Q64" s="32"/>
-      <c r="R64" s="32"/>
-      <c r="V64" s="32"/>
-      <c r="W64" s="32"/>
-      <c r="X64" s="32"/>
-      <c r="Y64" s="32"/>
+      <c r="P64" s="35"/>
+      <c r="Q64" s="35"/>
+      <c r="R64" s="35"/>
+      <c r="V64" s="35"/>
+      <c r="W64" s="35"/>
+      <c r="X64" s="35"/>
+      <c r="Y64" s="35"/>
     </row>
     <row r="65" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G65" s="32" t="s">
+      <c r="G65" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H65" s="32"/>
-      <c r="I65" s="32"/>
-      <c r="J65" s="32"/>
+      <c r="H65" s="35"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="35"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
       <c r="N65" s="18"/>
-      <c r="O65" s="32"/>
-      <c r="P65" s="32"/>
-      <c r="Q65" s="32"/>
-      <c r="R65" s="32"/>
-      <c r="V65" s="32"/>
-      <c r="W65" s="32"/>
-      <c r="X65" s="32"/>
-      <c r="Y65" s="32"/>
+      <c r="O65" s="35"/>
+      <c r="P65" s="35"/>
+      <c r="Q65" s="35"/>
+      <c r="R65" s="35"/>
+      <c r="V65" s="35"/>
+      <c r="W65" s="35"/>
+      <c r="X65" s="35"/>
+      <c r="Y65" s="35"/>
     </row>
     <row r="66" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="32"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
       <c r="K66" s="15"/>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
       <c r="N66" s="18"/>
-      <c r="O66" s="34" t="s">
+      <c r="O66" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="P66" s="34"/>
-      <c r="Q66" s="34"/>
-      <c r="R66" s="34"/>
-      <c r="V66" s="32" t="s">
+      <c r="P66" s="38"/>
+      <c r="Q66" s="38"/>
+      <c r="R66" s="38"/>
+      <c r="V66" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="W66" s="32"/>
-      <c r="X66" s="32"/>
-      <c r="Y66" s="32"/>
+      <c r="W66" s="35"/>
+      <c r="X66" s="35"/>
+      <c r="Y66" s="35"/>
     </row>
     <row r="67" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G67" s="32"/>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="32"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12"/>
       <c r="N67" s="18"/>
-      <c r="O67" s="34"/>
-      <c r="P67" s="34"/>
-      <c r="Q67" s="34"/>
-      <c r="R67" s="34"/>
-      <c r="V67" s="32"/>
-      <c r="W67" s="32"/>
-      <c r="X67" s="32"/>
-      <c r="Y67" s="32"/>
+      <c r="O67" s="38"/>
+      <c r="P67" s="38"/>
+      <c r="Q67" s="38"/>
+      <c r="R67" s="38"/>
+      <c r="V67" s="35"/>
+      <c r="W67" s="35"/>
+      <c r="X67" s="35"/>
+      <c r="Y67" s="35"/>
     </row>
     <row r="68" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O68" s="41" t="s">
+      <c r="O68" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="P68" s="30"/>
-      <c r="Q68" s="30"/>
-      <c r="R68" s="30"/>
-      <c r="V68" s="32"/>
-      <c r="W68" s="32"/>
-      <c r="X68" s="32"/>
-      <c r="Y68" s="32"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+      <c r="V68" s="35"/>
+      <c r="W68" s="35"/>
+      <c r="X68" s="35"/>
+      <c r="Y68" s="35"/>
     </row>
     <row r="69" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O69" s="30"/>
-      <c r="P69" s="30"/>
-      <c r="Q69" s="30"/>
-      <c r="R69" s="30"/>
-      <c r="V69" s="32"/>
-      <c r="W69" s="32"/>
-      <c r="X69" s="32"/>
-      <c r="Y69" s="32"/>
+      <c r="O69" s="37"/>
+      <c r="P69" s="37"/>
+      <c r="Q69" s="37"/>
+      <c r="R69" s="37"/>
+      <c r="V69" s="35"/>
+      <c r="W69" s="35"/>
+      <c r="X69" s="35"/>
+      <c r="Y69" s="35"/>
     </row>
     <row r="70" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O70" s="41" t="s">
+      <c r="O70" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="P70" s="41"/>
-      <c r="Q70" s="41"/>
-      <c r="R70" s="41"/>
-      <c r="S70" s="41"/>
-      <c r="V70" s="32"/>
-      <c r="W70" s="32"/>
-      <c r="X70" s="32"/>
-      <c r="Y70" s="32"/>
+      <c r="P70" s="36"/>
+      <c r="Q70" s="36"/>
+      <c r="R70" s="36"/>
+      <c r="S70" s="36"/>
+      <c r="V70" s="35"/>
+      <c r="W70" s="35"/>
+      <c r="X70" s="35"/>
+      <c r="Y70" s="35"/>
     </row>
     <row r="71" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O71" s="41"/>
-      <c r="P71" s="41"/>
-      <c r="Q71" s="41"/>
-      <c r="R71" s="41"/>
-      <c r="S71" s="41"/>
-      <c r="V71" s="32"/>
-      <c r="W71" s="32"/>
-      <c r="X71" s="32"/>
-      <c r="Y71" s="32"/>
+      <c r="O71" s="36"/>
+      <c r="P71" s="36"/>
+      <c r="Q71" s="36"/>
+      <c r="R71" s="36"/>
+      <c r="S71" s="36"/>
+      <c r="V71" s="35"/>
+      <c r="W71" s="35"/>
+      <c r="X71" s="35"/>
+      <c r="Y71" s="35"/>
     </row>
     <row r="72" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V72" s="31"/>
-      <c r="W72" s="32"/>
-      <c r="X72" s="32"/>
-      <c r="Y72" s="32"/>
+      <c r="V72" s="39"/>
+      <c r="W72" s="35"/>
+      <c r="X72" s="35"/>
+      <c r="Y72" s="35"/>
     </row>
     <row r="73" spans="7:25" x14ac:dyDescent="0.3">
       <c r="K73" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="V73" s="32"/>
-      <c r="W73" s="32"/>
-      <c r="X73" s="32"/>
-      <c r="Y73" s="32"/>
+      <c r="V73" s="35"/>
+      <c r="W73" s="35"/>
+      <c r="X73" s="35"/>
+      <c r="Y73" s="35"/>
     </row>
     <row r="74" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V74" s="32"/>
-      <c r="W74" s="32"/>
-      <c r="X74" s="32"/>
-      <c r="Y74" s="32"/>
+      <c r="V74" s="35"/>
+      <c r="W74" s="35"/>
+      <c r="X74" s="35"/>
+      <c r="Y74" s="35"/>
     </row>
     <row r="79" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V79" s="32" t="s">
+      <c r="V79" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="W79" s="32"/>
-      <c r="X79" s="32"/>
-      <c r="Y79" s="32"/>
+      <c r="W79" s="35"/>
+      <c r="X79" s="35"/>
+      <c r="Y79" s="35"/>
     </row>
     <row r="80" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="O80" s="32" t="s">
+      <c r="O80" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="P80" s="32"/>
-      <c r="Q80" s="32"/>
-      <c r="R80" s="32"/>
-      <c r="V80" s="32"/>
-      <c r="W80" s="32"/>
-      <c r="X80" s="32"/>
-      <c r="Y80" s="32"/>
+      <c r="P80" s="35"/>
+      <c r="Q80" s="35"/>
+      <c r="R80" s="35"/>
+      <c r="V80" s="35"/>
+      <c r="W80" s="35"/>
+      <c r="X80" s="35"/>
+      <c r="Y80" s="35"/>
     </row>
     <row r="81" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G81" s="32" t="s">
+      <c r="G81" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H81" s="32"/>
-      <c r="I81" s="32"/>
-      <c r="J81" s="32"/>
+      <c r="H81" s="35"/>
+      <c r="I81" s="35"/>
+      <c r="J81" s="35"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12"/>
       <c r="N81" s="18"/>
-      <c r="O81" s="32"/>
-      <c r="P81" s="32"/>
-      <c r="Q81" s="32"/>
-      <c r="R81" s="32"/>
-      <c r="V81" s="32"/>
-      <c r="W81" s="32"/>
-      <c r="X81" s="32"/>
-      <c r="Y81" s="32"/>
+      <c r="O81" s="35"/>
+      <c r="P81" s="35"/>
+      <c r="Q81" s="35"/>
+      <c r="R81" s="35"/>
+      <c r="V81" s="35"/>
+      <c r="W81" s="35"/>
+      <c r="X81" s="35"/>
+      <c r="Y81" s="35"/>
     </row>
     <row r="82" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G82" s="32"/>
-      <c r="H82" s="32"/>
-      <c r="I82" s="32"/>
-      <c r="J82" s="32"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="35"/>
+      <c r="J82" s="35"/>
       <c r="K82" s="15"/>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
       <c r="N82" s="18"/>
-      <c r="O82" s="34" t="s">
+      <c r="O82" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="P82" s="34"/>
-      <c r="Q82" s="34"/>
-      <c r="R82" s="34"/>
-      <c r="S82" s="40"/>
-      <c r="V82" s="32" t="s">
+      <c r="P82" s="38"/>
+      <c r="Q82" s="38"/>
+      <c r="R82" s="38"/>
+      <c r="S82" s="23"/>
+      <c r="V82" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="W82" s="32"/>
-      <c r="X82" s="32"/>
-      <c r="Y82" s="32"/>
+      <c r="W82" s="35"/>
+      <c r="X82" s="35"/>
+      <c r="Y82" s="35"/>
     </row>
     <row r="83" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G83" s="32"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32"/>
-      <c r="J83" s="32"/>
+      <c r="G83" s="35"/>
+      <c r="H83" s="35"/>
+      <c r="I83" s="35"/>
+      <c r="J83" s="35"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
       <c r="N83" s="18"/>
-      <c r="O83" s="34"/>
-      <c r="P83" s="34"/>
-      <c r="Q83" s="34"/>
-      <c r="R83" s="34"/>
-      <c r="S83" s="40"/>
-      <c r="T83" s="39"/>
-      <c r="U83" s="39"/>
-      <c r="V83" s="32"/>
-      <c r="W83" s="32"/>
-      <c r="X83" s="32"/>
-      <c r="Y83" s="32"/>
+      <c r="O83" s="38"/>
+      <c r="P83" s="38"/>
+      <c r="Q83" s="38"/>
+      <c r="R83" s="38"/>
+      <c r="S83" s="23"/>
+      <c r="T83" s="22"/>
+      <c r="U83" s="22"/>
+      <c r="V83" s="35"/>
+      <c r="W83" s="35"/>
+      <c r="X83" s="35"/>
+      <c r="Y83" s="35"/>
     </row>
     <row r="84" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="O84" s="41" t="s">
+      <c r="O84" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="P84" s="30"/>
-      <c r="Q84" s="30"/>
-      <c r="R84" s="30"/>
-      <c r="S84" s="40"/>
-      <c r="V84" s="32"/>
-      <c r="W84" s="32"/>
-      <c r="X84" s="32"/>
-      <c r="Y84" s="32"/>
+      <c r="P84" s="37"/>
+      <c r="Q84" s="37"/>
+      <c r="R84" s="37"/>
+      <c r="S84" s="23"/>
+      <c r="V84" s="35"/>
+      <c r="W84" s="35"/>
+      <c r="X84" s="35"/>
+      <c r="Y84" s="35"/>
     </row>
     <row r="85" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="O85" s="30"/>
-      <c r="P85" s="30"/>
-      <c r="Q85" s="30"/>
-      <c r="R85" s="30"/>
-      <c r="V85" s="32" t="s">
+      <c r="O85" s="37"/>
+      <c r="P85" s="37"/>
+      <c r="Q85" s="37"/>
+      <c r="R85" s="37"/>
+      <c r="V85" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="W85" s="32"/>
-      <c r="X85" s="32"/>
-      <c r="Y85" s="32"/>
+      <c r="W85" s="35"/>
+      <c r="X85" s="35"/>
+      <c r="Y85" s="35"/>
     </row>
     <row r="86" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O86" s="41" t="s">
+      <c r="O86" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="P86" s="30"/>
-      <c r="Q86" s="30"/>
-      <c r="R86" s="30"/>
-      <c r="S86" s="42"/>
-      <c r="V86" s="32"/>
-      <c r="W86" s="32"/>
-      <c r="X86" s="32"/>
-      <c r="Y86" s="32"/>
+      <c r="P86" s="37"/>
+      <c r="Q86" s="37"/>
+      <c r="R86" s="37"/>
+      <c r="S86" s="24"/>
+      <c r="V86" s="35"/>
+      <c r="W86" s="35"/>
+      <c r="X86" s="35"/>
+      <c r="Y86" s="35"/>
     </row>
     <row r="87" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O87" s="30"/>
-      <c r="P87" s="30"/>
-      <c r="Q87" s="30"/>
-      <c r="R87" s="30"/>
-      <c r="S87" s="42"/>
-      <c r="V87" s="32"/>
-      <c r="W87" s="32"/>
-      <c r="X87" s="32"/>
-      <c r="Y87" s="32"/>
+      <c r="O87" s="37"/>
+      <c r="P87" s="37"/>
+      <c r="Q87" s="37"/>
+      <c r="R87" s="37"/>
+      <c r="S87" s="24"/>
+      <c r="V87" s="35"/>
+      <c r="W87" s="35"/>
+      <c r="X87" s="35"/>
+      <c r="Y87" s="35"/>
     </row>
     <row r="88" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V88" s="32"/>
-      <c r="W88" s="32"/>
-      <c r="X88" s="32"/>
-      <c r="Y88" s="32"/>
+      <c r="V88" s="35"/>
+      <c r="W88" s="35"/>
+      <c r="X88" s="35"/>
+      <c r="Y88" s="35"/>
     </row>
     <row r="89" spans="7:25" x14ac:dyDescent="0.3">
       <c r="K89" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="V89" s="32"/>
-      <c r="W89" s="32"/>
-      <c r="X89" s="32"/>
-      <c r="Y89" s="32"/>
+      <c r="V89" s="35"/>
+      <c r="W89" s="35"/>
+      <c r="X89" s="35"/>
+      <c r="Y89" s="35"/>
     </row>
     <row r="90" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V90" s="32"/>
-      <c r="W90" s="32"/>
-      <c r="X90" s="32"/>
-      <c r="Y90" s="32"/>
+      <c r="V90" s="35"/>
+      <c r="W90" s="35"/>
+      <c r="X90" s="35"/>
+      <c r="Y90" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="V88:Y90"/>
-    <mergeCell ref="O86:R87"/>
-    <mergeCell ref="V79:Y81"/>
-    <mergeCell ref="O80:R81"/>
-    <mergeCell ref="G81:J83"/>
-    <mergeCell ref="O82:R83"/>
-    <mergeCell ref="V82:Y84"/>
-    <mergeCell ref="O84:R85"/>
-    <mergeCell ref="V85:Y87"/>
-    <mergeCell ref="G65:J67"/>
-    <mergeCell ref="V63:Y65"/>
-    <mergeCell ref="V66:Y68"/>
-    <mergeCell ref="V69:Y71"/>
-    <mergeCell ref="V72:Y74"/>
-    <mergeCell ref="O64:R65"/>
-    <mergeCell ref="O66:R67"/>
-    <mergeCell ref="O68:R69"/>
-    <mergeCell ref="O70:S71"/>
+    <mergeCell ref="U52:W53"/>
+    <mergeCell ref="O44:R46"/>
+    <mergeCell ref="X36:Y37"/>
+    <mergeCell ref="X39:AB40"/>
+    <mergeCell ref="O50:R51"/>
+    <mergeCell ref="X44:AA45"/>
+    <mergeCell ref="U48:W49"/>
+    <mergeCell ref="U50:W51"/>
+    <mergeCell ref="G36:J38"/>
+    <mergeCell ref="O30:R31"/>
+    <mergeCell ref="O35:R37"/>
+    <mergeCell ref="O38:R40"/>
+    <mergeCell ref="O41:R43"/>
+    <mergeCell ref="S5:U6"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="K9:M10"/>
+    <mergeCell ref="O9:Q10"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="K5:M6"/>
+    <mergeCell ref="O5:Q6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="G13:I14"/>
+    <mergeCell ref="K13:M14"/>
     <mergeCell ref="C25:E26"/>
     <mergeCell ref="G25:I26"/>
     <mergeCell ref="O13:Q14"/>
@@ -2983,36 +3351,24 @@
     <mergeCell ref="K17:M18"/>
     <mergeCell ref="O17:Q18"/>
     <mergeCell ref="S17:U18"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="C13:E14"/>
-    <mergeCell ref="G13:I14"/>
-    <mergeCell ref="K13:M14"/>
-    <mergeCell ref="S5:U6"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="K9:M10"/>
-    <mergeCell ref="O9:Q10"/>
-    <mergeCell ref="S9:U10"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="K5:M6"/>
-    <mergeCell ref="O5:Q6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="G36:J38"/>
-    <mergeCell ref="O30:R31"/>
-    <mergeCell ref="O35:R37"/>
-    <mergeCell ref="O38:R40"/>
-    <mergeCell ref="O41:R43"/>
-    <mergeCell ref="U52:W53"/>
-    <mergeCell ref="O44:R46"/>
-    <mergeCell ref="X36:Y37"/>
-    <mergeCell ref="X39:AB40"/>
-    <mergeCell ref="O50:R51"/>
-    <mergeCell ref="X44:AA45"/>
-    <mergeCell ref="U48:W49"/>
-    <mergeCell ref="U50:W51"/>
+    <mergeCell ref="G65:J67"/>
+    <mergeCell ref="V63:Y65"/>
+    <mergeCell ref="V66:Y68"/>
+    <mergeCell ref="V69:Y71"/>
+    <mergeCell ref="V72:Y74"/>
+    <mergeCell ref="O64:R65"/>
+    <mergeCell ref="O66:R67"/>
+    <mergeCell ref="O68:R69"/>
+    <mergeCell ref="O70:S71"/>
+    <mergeCell ref="V88:Y90"/>
+    <mergeCell ref="O86:R87"/>
+    <mergeCell ref="V79:Y81"/>
+    <mergeCell ref="O80:R81"/>
+    <mergeCell ref="G81:J83"/>
+    <mergeCell ref="O82:R83"/>
+    <mergeCell ref="V82:Y84"/>
+    <mergeCell ref="O84:R85"/>
+    <mergeCell ref="V85:Y87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3021,233 +3377,869 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E37153-5D58-49F3-A7E8-18914BA10F81}">
-  <dimension ref="C2:T16"/>
+  <dimension ref="C2:X49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.6" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="10" width="8.88671875" style="43"/>
-    <col min="11" max="11" width="15" style="43" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="43"/>
+    <col min="1" max="10" width="8.88671875" style="25"/>
+    <col min="11" max="11" width="15" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="23" width="8.88671875" style="25"/>
+    <col min="24" max="24" width="12" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45" t="s">
+      <c r="D4" s="52"/>
+      <c r="E4" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45" t="s">
+      <c r="F4" s="52"/>
+      <c r="G4" s="52" t="s">
         <v>91</v>
       </c>
       <c r="H4" s="53"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="54"/>
-      <c r="P4" s="47" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="49"/>
+      <c r="P4" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="51" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="48"/>
+      <c r="G5" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="K5" s="44"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="48" t="s">
+      <c r="H5" s="48"/>
+      <c r="K5" s="26"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45" t="s">
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="K6" s="44"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="50">
+      <c r="K6" s="26"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="56">
         <v>100</v>
       </c>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46">
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55">
         <v>0</v>
       </c>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="K7" s="44"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="50">
+      <c r="K7" s="26"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="56">
         <v>25</v>
       </c>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46">
+      <c r="Q7" s="55"/>
+      <c r="R7" s="55">
         <v>0</v>
       </c>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="H8" s="43">
+      <c r="H8" s="25">
         <v>100</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="25">
         <v>0</v>
       </c>
-      <c r="K8" s="44"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="50">
+      <c r="K8" s="26"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="56">
         <v>25</v>
       </c>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46">
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55">
         <v>15</v>
       </c>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="H9" s="43">
+      <c r="H9" s="25">
         <v>25</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="50">
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="56">
         <v>25</v>
       </c>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46">
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55">
         <v>30</v>
       </c>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="50">
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="56">
         <v>25</v>
       </c>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46">
+      <c r="Q10" s="55"/>
+      <c r="R10" s="55">
         <v>45</v>
       </c>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="L12" s="43" t="s">
+      <c r="L12" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="M12" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="P12" s="43">
+      <c r="P12" s="25">
         <v>100</v>
       </c>
-      <c r="Q12" s="43" t="s">
+      <c r="Q12" s="25" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="L13" s="43" t="s">
+      <c r="L13" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="M13" s="25" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="L14" s="43" t="s">
+      <c r="L14" s="25" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="L15" s="43" t="s">
+      <c r="L15" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="M15" s="25" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="L16" s="43" t="s">
+      <c r="L16" s="25" t="s">
         <v>107</v>
       </c>
     </row>
+    <row r="27" spans="3:24" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="C27" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C28" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="66"/>
+    </row>
+    <row r="29" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C29" s="67"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="61"/>
+      <c r="S29" s="61"/>
+      <c r="T29" s="61"/>
+      <c r="U29" s="68"/>
+    </row>
+    <row r="30" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C30" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="77"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" s="77"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="L30" s="77"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O30" s="48"/>
+      <c r="P30" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="S30" s="48"/>
+      <c r="T30" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="U30" s="78"/>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C31" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="59"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="60"/>
+      <c r="T31" s="58"/>
+      <c r="U31" s="69"/>
+      <c r="X31" s="87"/>
+    </row>
+    <row r="32" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C32" s="79"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" s="59"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="L32" s="59"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="O32" s="60"/>
+      <c r="P32" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="S32" s="60"/>
+      <c r="T32" s="58"/>
+      <c r="U32" s="69"/>
+      <c r="X32" s="25">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C33" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I33" s="59"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="60"/>
+      <c r="T33" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="U33" s="69"/>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C34" s="79">
+        <v>1</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="58">
+        <v>1</v>
+      </c>
+      <c r="F34" s="59"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="58">
+        <v>1</v>
+      </c>
+      <c r="I34" s="59"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="58">
+        <v>1</v>
+      </c>
+      <c r="L34" s="59"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="60"/>
+      <c r="T34" s="58">
+        <v>95</v>
+      </c>
+      <c r="U34" s="69"/>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C35" s="79">
+        <v>2</v>
+      </c>
+      <c r="D35" s="48"/>
+      <c r="E35" s="58">
+        <v>1</v>
+      </c>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="58">
+        <v>1</v>
+      </c>
+      <c r="I35" s="59"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="58">
+        <v>2</v>
+      </c>
+      <c r="L35" s="59"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="60"/>
+      <c r="T35" s="58">
+        <v>5</v>
+      </c>
+      <c r="U35" s="69"/>
+      <c r="W35" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C36" s="79">
+        <v>3</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="58">
+        <v>3</v>
+      </c>
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="58">
+        <v>1</v>
+      </c>
+      <c r="I36" s="59"/>
+      <c r="J36" s="60"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="58">
+        <v>11</v>
+      </c>
+      <c r="O36" s="60"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="58">
+        <v>100</v>
+      </c>
+      <c r="U36" s="69"/>
+    </row>
+    <row r="37" spans="3:24" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="C37" s="80">
+        <v>4</v>
+      </c>
+      <c r="D37" s="81"/>
+      <c r="E37" s="73">
+        <v>1</v>
+      </c>
+      <c r="F37" s="74"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="73">
+        <v>45</v>
+      </c>
+      <c r="I37" s="74"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="73">
+        <v>2</v>
+      </c>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="73">
+        <v>100</v>
+      </c>
+      <c r="U37" s="76"/>
+      <c r="X37" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="3:24" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7"/>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C40" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="62"/>
+      <c r="T40" s="62"/>
+      <c r="U40" s="62"/>
+    </row>
+    <row r="41" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C41" s="67"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="68"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="62"/>
+      <c r="M41" s="62"/>
+      <c r="N41" s="62"/>
+      <c r="O41" s="62"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="62"/>
+      <c r="R41" s="62"/>
+      <c r="S41" s="62"/>
+      <c r="T41" s="62"/>
+      <c r="U41" s="62"/>
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C42" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="77"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="I42" s="77"/>
+      <c r="J42" s="78"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="63"/>
+      <c r="U42" s="63"/>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C43" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="60"/>
+      <c r="E43" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="69"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="63"/>
+      <c r="S43" s="63"/>
+      <c r="T43" s="63"/>
+      <c r="U43" s="63"/>
+    </row>
+    <row r="44" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C44" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="60"/>
+      <c r="E44" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="59"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="69"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="63"/>
+      <c r="S44" s="63"/>
+      <c r="T44" s="63"/>
+      <c r="U44" s="63"/>
+    </row>
+    <row r="45" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C45" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="60"/>
+      <c r="E45" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="59"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I45" s="59"/>
+      <c r="J45" s="69"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="63"/>
+      <c r="R45" s="63"/>
+      <c r="S45" s="63"/>
+      <c r="T45" s="63"/>
+      <c r="U45" s="63"/>
+    </row>
+    <row r="46" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C46" s="70"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="63"/>
+      <c r="P46" s="63"/>
+      <c r="Q46" s="63"/>
+      <c r="R46" s="63"/>
+      <c r="S46" s="63"/>
+      <c r="T46" s="63"/>
+      <c r="U46" s="63"/>
+    </row>
+    <row r="47" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C47" s="70"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="63"/>
+      <c r="R47" s="63"/>
+      <c r="S47" s="63"/>
+      <c r="T47" s="63"/>
+      <c r="U47" s="63"/>
+    </row>
+    <row r="48" spans="3:24" x14ac:dyDescent="0.65">
+      <c r="C48" s="70"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="63"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="63"/>
+      <c r="O48" s="63"/>
+      <c r="P48" s="63"/>
+      <c r="Q48" s="63"/>
+      <c r="R48" s="63"/>
+      <c r="S48" s="63"/>
+      <c r="T48" s="63"/>
+      <c r="U48" s="63"/>
+    </row>
+    <row r="49" spans="3:21" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="C49" s="71"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="73"/>
+      <c r="I49" s="74"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+      <c r="O49" s="63"/>
+      <c r="P49" s="63"/>
+      <c r="Q49" s="63"/>
+      <c r="R49" s="63"/>
+      <c r="S49" s="63"/>
+      <c r="T49" s="63"/>
+      <c r="U49" s="63"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
+  <mergeCells count="118">
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C28:U29"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
     <mergeCell ref="M9:O9"/>
     <mergeCell ref="M10:O10"/>
     <mergeCell ref="P4:T4"/>
@@ -3264,14 +4256,13 @@
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:T5"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregar ER en drawio
</commit_message>
<xml_diff>
--- a/ER.xlsx
+++ b/ER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\GitHub\SBD1-Perfumeria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A8E1FD-9363-469D-B39B-189B7BE2874E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E18AAC2-8E5C-47A5-89C0-AD399AEF150F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E58047A2-82F4-49D8-8F0D-4EA110376B37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E58047A2-82F4-49D8-8F0D-4EA110376B37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,12 +498,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="5"/>
-      <name val="Roboto"/>
     </font>
     <font>
       <b/>
@@ -934,7 +928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1010,6 +1004,32 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1019,176 +1039,147 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1505,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075D56C9-9013-44E8-86C7-ACC885266A1C}">
   <dimension ref="C5:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -1517,377 +1508,377 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="I5" s="30" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="I5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="T5" s="30" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="T5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
+      <c r="U5" s="36"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="36"/>
     </row>
     <row r="6" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
     </row>
     <row r="7" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="I7" s="27" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="I7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29"/>
-      <c r="T7" s="32" t="s">
+      <c r="J7" s="38"/>
+      <c r="K7" s="39"/>
+      <c r="T7" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
     </row>
     <row r="8" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="I8" s="27" t="s">
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="I8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
-      <c r="T8" s="32" t="s">
+      <c r="J8" s="38"/>
+      <c r="K8" s="39"/>
+      <c r="T8" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29"/>
-      <c r="T9" s="32" t="s">
+      <c r="I9" s="37"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
+      <c r="T9" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
     </row>
     <row r="10" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="29"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="29"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="39"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
     </row>
     <row r="12" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="G12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
       <c r="G13" s="6"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
     </row>
     <row r="14" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
       <c r="G14" s="7"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
       <c r="G15" s="7"/>
-      <c r="U15" s="30" t="s">
+      <c r="U15" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
     </row>
     <row r="16" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
       <c r="G16" s="7"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
     </row>
     <row r="17" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="U17" s="27" t="s">
+      <c r="U17" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="V17" s="28"/>
-      <c r="W17" s="29"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="39"/>
     </row>
     <row r="18" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
       <c r="G18" s="7"/>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="O18" s="30" t="s">
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="O18" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="U18" s="27" t="s">
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="U18" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="V18" s="28"/>
-      <c r="W18" s="29"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="39"/>
     </row>
     <row r="19" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
       <c r="G19" s="7"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
       <c r="L19" s="3"/>
       <c r="M19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="N19" s="5"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
       <c r="V19" s="6"/>
     </row>
     <row r="20" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
       <c r="G20" s="7"/>
-      <c r="I20" s="33" t="s">
+      <c r="I20" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="O20" s="27" t="s">
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="O20" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="29"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="39"/>
       <c r="V20" s="3"/>
     </row>
     <row r="21" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
       <c r="G21" s="7"/>
-      <c r="I21" s="33" t="s">
+      <c r="I21" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="O21" s="27" t="s">
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="O21" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="29"/>
-      <c r="U21" s="30" t="s">
+      <c r="P21" s="38"/>
+      <c r="Q21" s="39"/>
+      <c r="U21" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
     </row>
     <row r="22" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="9"/>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="30"/>
-      <c r="W22" s="30"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="I23" s="33" t="s">
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
+      <c r="I23" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="U23" s="27" t="s">
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="U23" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="28"/>
-      <c r="W23" s="29"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="39"/>
     </row>
     <row r="24" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="I24" s="33" t="s">
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="I24" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="U24" s="27" t="s">
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="U24" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="V24" s="28"/>
-      <c r="W24" s="29"/>
+      <c r="V24" s="38"/>
+      <c r="W24" s="39"/>
     </row>
     <row r="25" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C25" s="27"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
-      <c r="I25" s="33" t="s">
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="I25" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C26" s="27"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
       <c r="V26" s="3"/>
     </row>
     <row r="27" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
-      <c r="U27" s="30" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
+      <c r="U27" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D28" s="6"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
+      <c r="U28" s="36"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="36"/>
     </row>
     <row r="29" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D29" s="7"/>
-      <c r="I29" s="30" t="s">
+      <c r="I29" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="U29" s="27" t="s">
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="U29" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="V29" s="28"/>
-      <c r="W29" s="29"/>
+      <c r="V29" s="38"/>
+      <c r="W29" s="39"/>
     </row>
     <row r="30" spans="3:23" x14ac:dyDescent="0.3">
       <c r="D30" s="3"/>
@@ -1897,94 +1888,117 @@
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="U30" s="27" t="s">
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="U30" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="V30" s="28"/>
-      <c r="W30" s="29"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="39"/>
     </row>
     <row r="31" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="I31" s="33" t="s">
+      <c r="I31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="U31" s="27" t="s">
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="U31" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="V31" s="28"/>
-      <c r="W31" s="29"/>
+      <c r="V31" s="38"/>
+      <c r="W31" s="39"/>
     </row>
     <row r="32" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
       <c r="V32" s="6"/>
     </row>
     <row r="33" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I33" s="34" t="s">
+      <c r="I33" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
       <c r="V33" s="3"/>
     </row>
     <row r="34" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="U34" s="30" t="s">
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="U34" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
+      <c r="V34" s="36"/>
+      <c r="W34" s="36"/>
     </row>
     <row r="35" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="U35" s="36"/>
+      <c r="V35" s="36"/>
+      <c r="W35" s="36"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="U36" s="27" t="s">
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="U36" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="V36" s="28"/>
-      <c r="W36" s="29"/>
+      <c r="V36" s="38"/>
+      <c r="W36" s="39"/>
     </row>
     <row r="37" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="U37" s="27" t="s">
+      <c r="U37" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="V37" s="28"/>
-      <c r="W37" s="29"/>
+      <c r="V37" s="38"/>
+      <c r="W37" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I5:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="U34:W35"/>
+    <mergeCell ref="U36:W36"/>
+    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="U21:W22"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="U27:W28"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="T5:W6"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="U15:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="I29:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="O18:Q19"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C26:E26"/>
@@ -2001,43 +2015,20 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="O18:Q19"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="T5:W6"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="U15:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="I29:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="U21:W22"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="U27:W28"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="U34:W35"/>
-    <mergeCell ref="U36:W36"/>
-    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2048,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A331C8E-6E8A-4DD1-B66D-75D29915EE06}">
   <dimension ref="C4:AB90"/>
   <sheetViews>
-    <sheetView topLeftCell="F29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N46" sqref="M46:N46"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2065,220 +2056,220 @@
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="K5" s="40" t="s">
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="K5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="O5" s="40" t="s">
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="O5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="S5" s="40" t="s">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="S5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
       <c r="V5" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
       <c r="V6" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="43" t="s">
+      <c r="S7" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
       <c r="V7" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="G9" s="41" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="G9" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="K9" s="41" t="s">
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="K9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="O9" s="40" t="s">
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="O9" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="S9" s="40" t="s">
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="S9" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
     </row>
     <row r="10" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="40"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="K11" s="43" t="s">
+      <c r="K11" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
     </row>
     <row r="13" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="G13" s="44" t="s">
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="G13" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="K13" s="41" t="s">
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="K13" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="O13" s="41" t="s">
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="O13" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="S13" s="41" t="s">
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="S13" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="G17" s="40" t="s">
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="G17" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="K17" s="40" t="s">
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="K17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="O17" s="41" t="s">
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="O17" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="S17" s="41" t="s">
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="S17" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="T17" s="41"/>
-      <c r="U17" s="41"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="41"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C19" s="11" t="s">
@@ -2286,60 +2277,60 @@
       </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="G21" s="40" t="s">
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="G21" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="K21" s="42" t="s">
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="K21" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="O21" s="41" t="s">
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="O21" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="S21" s="41" t="s">
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="S21" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="T21" s="41"/>
-      <c r="U21" s="41"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
-      <c r="U22" s="41"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
     </row>
     <row r="25" spans="3:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="G25" s="40" t="s">
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="G25" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
@@ -2356,12 +2347,12 @@
       <c r="AA25" s="10"/>
     </row>
     <row r="26" spans="3:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
@@ -2451,12 +2442,12 @@
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
       <c r="N30" s="10"/>
-      <c r="O30" s="35" t="s">
+      <c r="O30" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="35"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="10"/>
@@ -2476,10 +2467,10 @@
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="10"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="35"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
       <c r="U31" s="10"/>
@@ -2565,15 +2556,15 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="13"/>
-      <c r="L35" s="82"/>
+      <c r="L35" s="29"/>
       <c r="M35" s="12"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="35" t="s">
+      <c r="O35" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="35"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="10"/>
@@ -2585,68 +2576,68 @@
       <c r="AA35" s="10"/>
     </row>
     <row r="36" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="82"/>
+      <c r="L36" s="29"/>
       <c r="M36" s="12"/>
       <c r="N36" s="10"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="35"/>
+      <c r="O36" s="45"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="45"/>
+      <c r="R36" s="45"/>
       <c r="S36" s="13"/>
       <c r="T36" s="13"/>
       <c r="U36" s="10"/>
       <c r="V36" s="13"/>
       <c r="W36" s="12"/>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="45"/>
+      <c r="X36" s="46"/>
+      <c r="Y36" s="46"/>
       <c r="Z36" s="10"/>
       <c r="AA36" s="10"/>
     </row>
     <row r="37" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
       <c r="K37" s="15"/>
-      <c r="L37" s="82"/>
+      <c r="L37" s="29"/>
       <c r="M37" s="15"/>
       <c r="N37" s="18"/>
-      <c r="O37" s="35"/>
-      <c r="P37" s="35"/>
-      <c r="Q37" s="35"/>
-      <c r="R37" s="35"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
       <c r="U37" s="10"/>
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="46"/>
       <c r="Z37" s="10"/>
       <c r="AA37" s="10"/>
     </row>
     <row r="38" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="82"/>
+      <c r="L38" s="29"/>
       <c r="M38" s="12"/>
       <c r="N38" s="10"/>
-      <c r="O38" s="35" t="s">
+      <c r="O38" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="35"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="45"/>
       <c r="S38" s="13"/>
       <c r="T38" s="13"/>
       <c r="U38" s="10"/>
@@ -2663,23 +2654,23 @@
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="82"/>
+      <c r="L39" s="29"/>
       <c r="M39" s="12"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
       <c r="U39" s="10"/>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
-      <c r="X39" s="45"/>
-      <c r="Y39" s="45"/>
-      <c r="Z39" s="45"/>
-      <c r="AA39" s="45"/>
-      <c r="AB39" s="45"/>
+      <c r="X39" s="46"/>
+      <c r="Y39" s="46"/>
+      <c r="Z39" s="46"/>
+      <c r="AA39" s="46"/>
+      <c r="AB39" s="46"/>
     </row>
     <row r="40" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G40" s="10"/>
@@ -2690,20 +2681,20 @@
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
       <c r="N40" s="10"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
       <c r="U40" s="10"/>
       <c r="V40" s="13"/>
       <c r="W40" s="12"/>
-      <c r="X40" s="45"/>
-      <c r="Y40" s="45"/>
-      <c r="Z40" s="45"/>
-      <c r="AA40" s="45"/>
-      <c r="AB40" s="45"/>
+      <c r="X40" s="46"/>
+      <c r="Y40" s="46"/>
+      <c r="Z40" s="46"/>
+      <c r="AA40" s="46"/>
+      <c r="AB40" s="46"/>
     </row>
     <row r="41" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="10"/>
@@ -2714,12 +2705,12 @@
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
       <c r="N41" s="10"/>
-      <c r="O41" s="35" t="s">
+      <c r="O41" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
+      <c r="P41" s="45"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
       <c r="U41" s="10"/>
@@ -2739,10 +2730,10 @@
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
       <c r="N42" s="10"/>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="35"/>
+      <c r="O42" s="45"/>
+      <c r="P42" s="45"/>
+      <c r="Q42" s="45"/>
+      <c r="R42" s="45"/>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
       <c r="U42" s="10"/>
@@ -2762,10 +2753,10 @@
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
       <c r="N43" s="10"/>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="35"/>
+      <c r="O43" s="45"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
       <c r="U43" s="10"/>
@@ -2777,7 +2768,7 @@
       <c r="AA43" s="10"/>
     </row>
     <row r="44" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G44" s="83"/>
+      <c r="G44" s="30"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
@@ -2785,24 +2776,24 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="35"/>
-      <c r="Q44" s="35"/>
-      <c r="R44" s="35"/>
+      <c r="O44" s="44"/>
+      <c r="P44" s="45"/>
+      <c r="Q44" s="45"/>
+      <c r="R44" s="45"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
       <c r="U44" s="10"/>
       <c r="V44" s="13"/>
       <c r="W44" s="12"/>
-      <c r="X44" s="35" t="s">
+      <c r="X44" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="Y44" s="35"/>
-      <c r="Z44" s="35"/>
-      <c r="AA44" s="35"/>
+      <c r="Y44" s="45"/>
+      <c r="Z44" s="45"/>
+      <c r="AA44" s="45"/>
     </row>
     <row r="45" spans="7:28" x14ac:dyDescent="0.3">
-      <c r="G45" s="83" t="s">
+      <c r="G45" s="30" t="s">
         <v>123</v>
       </c>
       <c r="H45" s="10"/>
@@ -2812,35 +2803,35 @@
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
-      <c r="O45" s="35"/>
-      <c r="P45" s="35"/>
-      <c r="Q45" s="35"/>
-      <c r="R45" s="35"/>
+      <c r="O45" s="45"/>
+      <c r="P45" s="45"/>
+      <c r="Q45" s="45"/>
+      <c r="R45" s="45"/>
       <c r="S45" s="16"/>
       <c r="T45" s="16"/>
       <c r="U45" s="16"/>
       <c r="V45" s="12"/>
       <c r="W45" s="15"/>
-      <c r="X45" s="35"/>
-      <c r="Y45" s="35"/>
-      <c r="Z45" s="35"/>
-      <c r="AA45" s="35"/>
+      <c r="X45" s="45"/>
+      <c r="Y45" s="45"/>
+      <c r="Z45" s="45"/>
+      <c r="AA45" s="45"/>
     </row>
     <row r="46" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G46" s="83" t="s">
+      <c r="G46" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="H46" s="83"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="83"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="83"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="35"/>
+      <c r="O46" s="45"/>
+      <c r="P46" s="45"/>
+      <c r="Q46" s="45"/>
+      <c r="R46" s="45"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
       <c r="U46" s="16"/>
@@ -2852,14 +2843,14 @@
       <c r="AA46" s="10"/>
     </row>
     <row r="47" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G47" s="86" t="s">
+      <c r="G47" s="33" t="s">
         <v>125</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="10"/>
-      <c r="L47" s="83"/>
+      <c r="L47" s="30"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
@@ -2877,14 +2868,14 @@
       <c r="AA47" s="10"/>
     </row>
     <row r="48" spans="7:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="85" t="s">
+      <c r="G48" s="32" t="s">
         <v>126</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="10"/>
-      <c r="L48" s="83"/>
+      <c r="L48" s="30"/>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
@@ -2893,23 +2884,23 @@
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
-      <c r="U48" s="35" t="s">
+      <c r="U48" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="V48" s="35"/>
-      <c r="W48" s="35"/>
+      <c r="V48" s="45"/>
+      <c r="W48" s="45"/>
       <c r="X48" s="10"/>
       <c r="Y48" s="10"/>
       <c r="Z48" s="10"/>
       <c r="AA48" s="10"/>
     </row>
     <row r="49" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G49" s="84"/>
+      <c r="G49" s="31"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="10"/>
-      <c r="L49" s="83"/>
+      <c r="L49" s="30"/>
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
@@ -2918,9 +2909,9 @@
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
-      <c r="U49" s="35"/>
-      <c r="V49" s="35"/>
-      <c r="W49" s="35"/>
+      <c r="U49" s="45"/>
+      <c r="V49" s="45"/>
+      <c r="W49" s="45"/>
       <c r="X49" s="10"/>
       <c r="Y49" s="10"/>
       <c r="Z49" s="10"/>
@@ -2932,22 +2923,22 @@
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
       <c r="K50" s="10"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="83"/>
-      <c r="N50" s="83"/>
-      <c r="O50" s="35" t="s">
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
+      <c r="N50" s="30"/>
+      <c r="O50" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="P50" s="35"/>
-      <c r="Q50" s="35"/>
-      <c r="R50" s="35"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="45"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
-      <c r="U50" s="38" t="s">
+      <c r="U50" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="V50" s="38"/>
-      <c r="W50" s="38"/>
+      <c r="V50" s="47"/>
+      <c r="W50" s="47"/>
       <c r="X50" s="10"/>
       <c r="Y50" s="10"/>
       <c r="Z50" s="10"/>
@@ -2961,13 +2952,13 @@
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
-      <c r="O51" s="35"/>
-      <c r="P51" s="35"/>
-      <c r="Q51" s="35"/>
-      <c r="R51" s="35"/>
-      <c r="U51" s="38"/>
-      <c r="V51" s="38"/>
-      <c r="W51" s="38"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="45"/>
+      <c r="R51" s="45"/>
+      <c r="U51" s="47"/>
+      <c r="V51" s="47"/>
+      <c r="W51" s="47"/>
     </row>
     <row r="52" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G52" s="13"/>
@@ -2977,11 +2968,11 @@
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
-      <c r="U52" s="37" t="s">
+      <c r="U52" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="V52" s="37"/>
-      <c r="W52" s="37"/>
+      <c r="V52" s="43"/>
+      <c r="W52" s="43"/>
     </row>
     <row r="53" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G53" s="13"/>
@@ -2991,9 +2982,9 @@
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
-      <c r="U53" s="37"/>
-      <c r="V53" s="37"/>
-      <c r="W53" s="37"/>
+      <c r="U53" s="43"/>
+      <c r="V53" s="43"/>
+      <c r="W53" s="43"/>
     </row>
     <row r="54" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G54" s="13"/>
@@ -3005,338 +2996,326 @@
       <c r="M54" s="10"/>
     </row>
     <row r="63" spans="7:27" x14ac:dyDescent="0.3">
-      <c r="V63" s="35" t="s">
+      <c r="V63" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
-      <c r="Y63" s="35"/>
+      <c r="W63" s="45"/>
+      <c r="X63" s="45"/>
+      <c r="Y63" s="45"/>
     </row>
     <row r="64" spans="7:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O64" s="35" t="s">
+      <c r="O64" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="35"/>
-      <c r="V64" s="35"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
-      <c r="Y64" s="35"/>
+      <c r="P64" s="45"/>
+      <c r="Q64" s="45"/>
+      <c r="R64" s="45"/>
+      <c r="V64" s="45"/>
+      <c r="W64" s="45"/>
+      <c r="X64" s="45"/>
+      <c r="Y64" s="45"/>
     </row>
     <row r="65" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G65" s="35" t="s">
+      <c r="G65" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="45"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
       <c r="N65" s="18"/>
-      <c r="O65" s="35"/>
-      <c r="P65" s="35"/>
-      <c r="Q65" s="35"/>
-      <c r="R65" s="35"/>
-      <c r="V65" s="35"/>
-      <c r="W65" s="35"/>
-      <c r="X65" s="35"/>
-      <c r="Y65" s="35"/>
+      <c r="O65" s="45"/>
+      <c r="P65" s="45"/>
+      <c r="Q65" s="45"/>
+      <c r="R65" s="45"/>
+      <c r="V65" s="45"/>
+      <c r="W65" s="45"/>
+      <c r="X65" s="45"/>
+      <c r="Y65" s="45"/>
     </row>
     <row r="66" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
+      <c r="J66" s="45"/>
       <c r="K66" s="15"/>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
       <c r="N66" s="18"/>
-      <c r="O66" s="38" t="s">
+      <c r="O66" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="P66" s="38"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="38"/>
-      <c r="V66" s="35" t="s">
+      <c r="P66" s="47"/>
+      <c r="Q66" s="47"/>
+      <c r="R66" s="47"/>
+      <c r="V66" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="W66" s="35"/>
-      <c r="X66" s="35"/>
-      <c r="Y66" s="35"/>
+      <c r="W66" s="45"/>
+      <c r="X66" s="45"/>
+      <c r="Y66" s="45"/>
     </row>
     <row r="67" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="45"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12"/>
       <c r="N67" s="18"/>
-      <c r="O67" s="38"/>
-      <c r="P67" s="38"/>
-      <c r="Q67" s="38"/>
-      <c r="R67" s="38"/>
-      <c r="V67" s="35"/>
-      <c r="W67" s="35"/>
-      <c r="X67" s="35"/>
-      <c r="Y67" s="35"/>
+      <c r="O67" s="47"/>
+      <c r="P67" s="47"/>
+      <c r="Q67" s="47"/>
+      <c r="R67" s="47"/>
+      <c r="V67" s="45"/>
+      <c r="W67" s="45"/>
+      <c r="X67" s="45"/>
+      <c r="Y67" s="45"/>
     </row>
     <row r="68" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O68" s="36" t="s">
+      <c r="O68" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="P68" s="37"/>
-      <c r="Q68" s="37"/>
-      <c r="R68" s="37"/>
-      <c r="V68" s="35"/>
-      <c r="W68" s="35"/>
-      <c r="X68" s="35"/>
-      <c r="Y68" s="35"/>
+      <c r="P68" s="43"/>
+      <c r="Q68" s="43"/>
+      <c r="R68" s="43"/>
+      <c r="V68" s="45"/>
+      <c r="W68" s="45"/>
+      <c r="X68" s="45"/>
+      <c r="Y68" s="45"/>
     </row>
     <row r="69" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O69" s="37"/>
-      <c r="P69" s="37"/>
-      <c r="Q69" s="37"/>
-      <c r="R69" s="37"/>
-      <c r="V69" s="35"/>
-      <c r="W69" s="35"/>
-      <c r="X69" s="35"/>
-      <c r="Y69" s="35"/>
+      <c r="O69" s="43"/>
+      <c r="P69" s="43"/>
+      <c r="Q69" s="43"/>
+      <c r="R69" s="43"/>
+      <c r="V69" s="45"/>
+      <c r="W69" s="45"/>
+      <c r="X69" s="45"/>
+      <c r="Y69" s="45"/>
     </row>
     <row r="70" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O70" s="36" t="s">
+      <c r="O70" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="P70" s="36"/>
-      <c r="Q70" s="36"/>
-      <c r="R70" s="36"/>
-      <c r="S70" s="36"/>
-      <c r="V70" s="35"/>
-      <c r="W70" s="35"/>
-      <c r="X70" s="35"/>
-      <c r="Y70" s="35"/>
+      <c r="P70" s="52"/>
+      <c r="Q70" s="52"/>
+      <c r="R70" s="52"/>
+      <c r="S70" s="52"/>
+      <c r="V70" s="45"/>
+      <c r="W70" s="45"/>
+      <c r="X70" s="45"/>
+      <c r="Y70" s="45"/>
     </row>
     <row r="71" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O71" s="36"/>
-      <c r="P71" s="36"/>
-      <c r="Q71" s="36"/>
-      <c r="R71" s="36"/>
-      <c r="S71" s="36"/>
-      <c r="V71" s="35"/>
-      <c r="W71" s="35"/>
-      <c r="X71" s="35"/>
-      <c r="Y71" s="35"/>
+      <c r="O71" s="52"/>
+      <c r="P71" s="52"/>
+      <c r="Q71" s="52"/>
+      <c r="R71" s="52"/>
+      <c r="S71" s="52"/>
+      <c r="V71" s="45"/>
+      <c r="W71" s="45"/>
+      <c r="X71" s="45"/>
+      <c r="Y71" s="45"/>
     </row>
     <row r="72" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V72" s="39"/>
-      <c r="W72" s="35"/>
-      <c r="X72" s="35"/>
-      <c r="Y72" s="35"/>
+      <c r="V72" s="44"/>
+      <c r="W72" s="45"/>
+      <c r="X72" s="45"/>
+      <c r="Y72" s="45"/>
     </row>
     <row r="73" spans="7:25" x14ac:dyDescent="0.3">
       <c r="K73" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="V73" s="35"/>
-      <c r="W73" s="35"/>
-      <c r="X73" s="35"/>
-      <c r="Y73" s="35"/>
+      <c r="V73" s="45"/>
+      <c r="W73" s="45"/>
+      <c r="X73" s="45"/>
+      <c r="Y73" s="45"/>
     </row>
     <row r="74" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V74" s="35"/>
-      <c r="W74" s="35"/>
-      <c r="X74" s="35"/>
-      <c r="Y74" s="35"/>
+      <c r="V74" s="45"/>
+      <c r="W74" s="45"/>
+      <c r="X74" s="45"/>
+      <c r="Y74" s="45"/>
     </row>
     <row r="79" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V79" s="35" t="s">
+      <c r="V79" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="W79" s="35"/>
-      <c r="X79" s="35"/>
-      <c r="Y79" s="35"/>
+      <c r="W79" s="45"/>
+      <c r="X79" s="45"/>
+      <c r="Y79" s="45"/>
     </row>
     <row r="80" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="O80" s="35" t="s">
+      <c r="O80" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="P80" s="35"/>
-      <c r="Q80" s="35"/>
-      <c r="R80" s="35"/>
-      <c r="V80" s="35"/>
-      <c r="W80" s="35"/>
-      <c r="X80" s="35"/>
-      <c r="Y80" s="35"/>
+      <c r="P80" s="45"/>
+      <c r="Q80" s="45"/>
+      <c r="R80" s="45"/>
+      <c r="V80" s="45"/>
+      <c r="W80" s="45"/>
+      <c r="X80" s="45"/>
+      <c r="Y80" s="45"/>
     </row>
     <row r="81" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G81" s="35" t="s">
+      <c r="G81" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="H81" s="35"/>
-      <c r="I81" s="35"/>
-      <c r="J81" s="35"/>
+      <c r="H81" s="45"/>
+      <c r="I81" s="45"/>
+      <c r="J81" s="45"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12"/>
       <c r="N81" s="18"/>
-      <c r="O81" s="35"/>
-      <c r="P81" s="35"/>
-      <c r="Q81" s="35"/>
-      <c r="R81" s="35"/>
-      <c r="V81" s="35"/>
-      <c r="W81" s="35"/>
-      <c r="X81" s="35"/>
-      <c r="Y81" s="35"/>
+      <c r="O81" s="45"/>
+      <c r="P81" s="45"/>
+      <c r="Q81" s="45"/>
+      <c r="R81" s="45"/>
+      <c r="V81" s="45"/>
+      <c r="W81" s="45"/>
+      <c r="X81" s="45"/>
+      <c r="Y81" s="45"/>
     </row>
     <row r="82" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G82" s="35"/>
-      <c r="H82" s="35"/>
-      <c r="I82" s="35"/>
-      <c r="J82" s="35"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+      <c r="J82" s="45"/>
       <c r="K82" s="15"/>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
       <c r="N82" s="18"/>
-      <c r="O82" s="38" t="s">
+      <c r="O82" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="P82" s="38"/>
-      <c r="Q82" s="38"/>
-      <c r="R82" s="38"/>
+      <c r="P82" s="47"/>
+      <c r="Q82" s="47"/>
+      <c r="R82" s="47"/>
       <c r="S82" s="23"/>
-      <c r="V82" s="35" t="s">
+      <c r="V82" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="W82" s="35"/>
-      <c r="X82" s="35"/>
-      <c r="Y82" s="35"/>
+      <c r="W82" s="45"/>
+      <c r="X82" s="45"/>
+      <c r="Y82" s="45"/>
     </row>
     <row r="83" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G83" s="35"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="35"/>
-      <c r="J83" s="35"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="45"/>
+      <c r="I83" s="45"/>
+      <c r="J83" s="45"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
       <c r="N83" s="18"/>
-      <c r="O83" s="38"/>
-      <c r="P83" s="38"/>
-      <c r="Q83" s="38"/>
-      <c r="R83" s="38"/>
+      <c r="O83" s="47"/>
+      <c r="P83" s="47"/>
+      <c r="Q83" s="47"/>
+      <c r="R83" s="47"/>
       <c r="S83" s="23"/>
       <c r="T83" s="22"/>
       <c r="U83" s="22"/>
-      <c r="V83" s="35"/>
-      <c r="W83" s="35"/>
-      <c r="X83" s="35"/>
-      <c r="Y83" s="35"/>
+      <c r="V83" s="45"/>
+      <c r="W83" s="45"/>
+      <c r="X83" s="45"/>
+      <c r="Y83" s="45"/>
     </row>
     <row r="84" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="O84" s="36" t="s">
+      <c r="O84" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="P84" s="37"/>
-      <c r="Q84" s="37"/>
-      <c r="R84" s="37"/>
+      <c r="P84" s="43"/>
+      <c r="Q84" s="43"/>
+      <c r="R84" s="43"/>
       <c r="S84" s="23"/>
-      <c r="V84" s="35"/>
-      <c r="W84" s="35"/>
-      <c r="X84" s="35"/>
-      <c r="Y84" s="35"/>
+      <c r="V84" s="45"/>
+      <c r="W84" s="45"/>
+      <c r="X84" s="45"/>
+      <c r="Y84" s="45"/>
     </row>
     <row r="85" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="O85" s="37"/>
-      <c r="P85" s="37"/>
-      <c r="Q85" s="37"/>
-      <c r="R85" s="37"/>
-      <c r="V85" s="35" t="s">
+      <c r="O85" s="43"/>
+      <c r="P85" s="43"/>
+      <c r="Q85" s="43"/>
+      <c r="R85" s="43"/>
+      <c r="V85" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="W85" s="35"/>
-      <c r="X85" s="35"/>
-      <c r="Y85" s="35"/>
+      <c r="W85" s="45"/>
+      <c r="X85" s="45"/>
+      <c r="Y85" s="45"/>
     </row>
     <row r="86" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O86" s="36" t="s">
+      <c r="O86" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="P86" s="37"/>
-      <c r="Q86" s="37"/>
-      <c r="R86" s="37"/>
+      <c r="P86" s="43"/>
+      <c r="Q86" s="43"/>
+      <c r="R86" s="43"/>
       <c r="S86" s="24"/>
-      <c r="V86" s="35"/>
-      <c r="W86" s="35"/>
-      <c r="X86" s="35"/>
-      <c r="Y86" s="35"/>
+      <c r="V86" s="45"/>
+      <c r="W86" s="45"/>
+      <c r="X86" s="45"/>
+      <c r="Y86" s="45"/>
     </row>
     <row r="87" spans="7:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O87" s="37"/>
-      <c r="P87" s="37"/>
-      <c r="Q87" s="37"/>
-      <c r="R87" s="37"/>
+      <c r="O87" s="43"/>
+      <c r="P87" s="43"/>
+      <c r="Q87" s="43"/>
+      <c r="R87" s="43"/>
       <c r="S87" s="24"/>
-      <c r="V87" s="35"/>
-      <c r="W87" s="35"/>
-      <c r="X87" s="35"/>
-      <c r="Y87" s="35"/>
+      <c r="V87" s="45"/>
+      <c r="W87" s="45"/>
+      <c r="X87" s="45"/>
+      <c r="Y87" s="45"/>
     </row>
     <row r="88" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V88" s="35"/>
-      <c r="W88" s="35"/>
-      <c r="X88" s="35"/>
-      <c r="Y88" s="35"/>
+      <c r="V88" s="45"/>
+      <c r="W88" s="45"/>
+      <c r="X88" s="45"/>
+      <c r="Y88" s="45"/>
     </row>
     <row r="89" spans="7:25" x14ac:dyDescent="0.3">
       <c r="K89" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="V89" s="35"/>
-      <c r="W89" s="35"/>
-      <c r="X89" s="35"/>
-      <c r="Y89" s="35"/>
+      <c r="V89" s="45"/>
+      <c r="W89" s="45"/>
+      <c r="X89" s="45"/>
+      <c r="Y89" s="45"/>
     </row>
     <row r="90" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="V90" s="35"/>
-      <c r="W90" s="35"/>
-      <c r="X90" s="35"/>
-      <c r="Y90" s="35"/>
+      <c r="V90" s="45"/>
+      <c r="W90" s="45"/>
+      <c r="X90" s="45"/>
+      <c r="Y90" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="U52:W53"/>
-    <mergeCell ref="O44:R46"/>
-    <mergeCell ref="X36:Y37"/>
-    <mergeCell ref="X39:AB40"/>
-    <mergeCell ref="O50:R51"/>
-    <mergeCell ref="X44:AA45"/>
-    <mergeCell ref="U48:W49"/>
-    <mergeCell ref="U50:W51"/>
-    <mergeCell ref="G36:J38"/>
-    <mergeCell ref="O30:R31"/>
-    <mergeCell ref="O35:R37"/>
-    <mergeCell ref="O38:R40"/>
-    <mergeCell ref="O41:R43"/>
-    <mergeCell ref="S5:U6"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="K9:M10"/>
-    <mergeCell ref="O9:Q10"/>
-    <mergeCell ref="S9:U10"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="K5:M6"/>
-    <mergeCell ref="O5:Q6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="C13:E14"/>
-    <mergeCell ref="G13:I14"/>
-    <mergeCell ref="K13:M14"/>
+    <mergeCell ref="V88:Y90"/>
+    <mergeCell ref="O86:R87"/>
+    <mergeCell ref="V79:Y81"/>
+    <mergeCell ref="O80:R81"/>
+    <mergeCell ref="G81:J83"/>
+    <mergeCell ref="O82:R83"/>
+    <mergeCell ref="V82:Y84"/>
+    <mergeCell ref="O84:R85"/>
+    <mergeCell ref="V85:Y87"/>
+    <mergeCell ref="G65:J67"/>
+    <mergeCell ref="V63:Y65"/>
+    <mergeCell ref="V66:Y68"/>
+    <mergeCell ref="V69:Y71"/>
+    <mergeCell ref="V72:Y74"/>
+    <mergeCell ref="O64:R65"/>
+    <mergeCell ref="O66:R67"/>
+    <mergeCell ref="O68:R69"/>
+    <mergeCell ref="O70:S71"/>
     <mergeCell ref="C25:E26"/>
     <mergeCell ref="G25:I26"/>
     <mergeCell ref="O13:Q14"/>
@@ -3351,24 +3330,36 @@
     <mergeCell ref="K17:M18"/>
     <mergeCell ref="O17:Q18"/>
     <mergeCell ref="S17:U18"/>
-    <mergeCell ref="G65:J67"/>
-    <mergeCell ref="V63:Y65"/>
-    <mergeCell ref="V66:Y68"/>
-    <mergeCell ref="V69:Y71"/>
-    <mergeCell ref="V72:Y74"/>
-    <mergeCell ref="O64:R65"/>
-    <mergeCell ref="O66:R67"/>
-    <mergeCell ref="O68:R69"/>
-    <mergeCell ref="O70:S71"/>
-    <mergeCell ref="V88:Y90"/>
-    <mergeCell ref="O86:R87"/>
-    <mergeCell ref="V79:Y81"/>
-    <mergeCell ref="O80:R81"/>
-    <mergeCell ref="G81:J83"/>
-    <mergeCell ref="O82:R83"/>
-    <mergeCell ref="V82:Y84"/>
-    <mergeCell ref="O84:R85"/>
-    <mergeCell ref="V85:Y87"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="G13:I14"/>
+    <mergeCell ref="K13:M14"/>
+    <mergeCell ref="S5:U6"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="K9:M10"/>
+    <mergeCell ref="O9:Q10"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="K5:M6"/>
+    <mergeCell ref="O5:Q6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="G36:J38"/>
+    <mergeCell ref="O30:R31"/>
+    <mergeCell ref="O35:R37"/>
+    <mergeCell ref="O38:R40"/>
+    <mergeCell ref="O41:R43"/>
+    <mergeCell ref="U52:W53"/>
+    <mergeCell ref="O44:R46"/>
+    <mergeCell ref="X36:Y37"/>
+    <mergeCell ref="X39:AB40"/>
+    <mergeCell ref="O50:R51"/>
+    <mergeCell ref="X44:AA45"/>
+    <mergeCell ref="U48:W49"/>
+    <mergeCell ref="U50:W51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3379,7 +3370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E37153-5D58-49F3-A7E8-18914BA10F81}">
   <dimension ref="C2:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
@@ -3393,104 +3384,104 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52" t="s">
+      <c r="D4" s="82"/>
+      <c r="E4" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="49"/>
-      <c r="P4" s="51" t="s">
+      <c r="H4" s="83"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="79"/>
+      <c r="P4" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47" t="s">
+      <c r="D5" s="71"/>
+      <c r="E5" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="47" t="s">
+      <c r="F5" s="71"/>
+      <c r="G5" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="71"/>
       <c r="K5" s="26"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="57" t="s">
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52" t="s">
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82" t="s">
         <v>87</v>
       </c>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
+      <c r="S5" s="82"/>
+      <c r="T5" s="82"/>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.65">
       <c r="K6" s="26"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="56">
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="78">
         <v>100</v>
       </c>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55">
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77">
         <v>0</v>
       </c>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.65">
       <c r="K7" s="26"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="56">
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="78">
         <v>25</v>
       </c>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55">
+      <c r="Q7" s="77"/>
+      <c r="R7" s="77">
         <v>0</v>
       </c>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="77"/>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.65">
       <c r="H8" s="25">
@@ -3500,18 +3491,18 @@
         <v>0</v>
       </c>
       <c r="K8" s="26"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="56">
+      <c r="M8" s="79"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="78">
         <v>25</v>
       </c>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55">
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77">
         <v>15</v>
       </c>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
+      <c r="S8" s="77"/>
+      <c r="T8" s="77"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.65">
       <c r="H9" s="25">
@@ -3520,32 +3511,32 @@
       <c r="J9" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="56">
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="78">
         <v>25</v>
       </c>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55">
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77">
         <v>30</v>
       </c>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
+      <c r="S9" s="77"/>
+      <c r="T9" s="77"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.65">
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="56">
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="78">
         <v>25</v>
       </c>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="55">
+      <c r="Q10" s="77"/>
+      <c r="R10" s="77">
         <v>45</v>
       </c>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
+      <c r="S10" s="77"/>
+      <c r="T10" s="77"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.65">
       <c r="G12" s="25" t="s">
@@ -3605,237 +3596,237 @@
       </c>
     </row>
     <row r="28" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="65"/>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="65"/>
-      <c r="R28" s="65"/>
-      <c r="S28" s="65"/>
-      <c r="T28" s="65"/>
-      <c r="U28" s="66"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="54"/>
+      <c r="U28" s="55"/>
     </row>
     <row r="29" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C29" s="67"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="61"/>
-      <c r="P29" s="61"/>
-      <c r="Q29" s="61"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="68"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="57"/>
+      <c r="U29" s="58"/>
     </row>
     <row r="30" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C30" s="79" t="s">
+      <c r="C30" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="47" t="s">
+      <c r="D30" s="71"/>
+      <c r="E30" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="77"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="47" t="s">
+      <c r="F30" s="73"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="I30" s="77"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="47" t="s">
+      <c r="I30" s="73"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="L30" s="77"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="47" t="s">
+      <c r="L30" s="73"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="O30" s="48"/>
-      <c r="P30" s="47" t="s">
+      <c r="O30" s="71"/>
+      <c r="P30" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="47" t="s">
+      <c r="Q30" s="71"/>
+      <c r="R30" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="S30" s="48"/>
-      <c r="T30" s="47" t="s">
+      <c r="S30" s="71"/>
+      <c r="T30" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="U30" s="78"/>
+      <c r="U30" s="74"/>
     </row>
     <row r="31" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="58" t="s">
+      <c r="D31" s="71"/>
+      <c r="E31" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="F31" s="59"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="58" t="s">
+      <c r="F31" s="68"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="I31" s="59"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="60"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="60"/>
-      <c r="T31" s="58"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="67"/>
       <c r="U31" s="69"/>
-      <c r="X31" s="87"/>
+      <c r="X31" s="34"/>
     </row>
     <row r="32" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C32" s="79"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="58" t="s">
+      <c r="C32" s="70"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="58" t="s">
+      <c r="F32" s="68"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="59"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="58" t="s">
+      <c r="I32" s="68"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="L32" s="59"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="58" t="s">
+      <c r="L32" s="68"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="O32" s="60"/>
-      <c r="P32" s="58" t="s">
+      <c r="O32" s="66"/>
+      <c r="P32" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="58" t="s">
+      <c r="Q32" s="66"/>
+      <c r="R32" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="S32" s="60"/>
-      <c r="T32" s="58"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="67"/>
       <c r="U32" s="69"/>
       <c r="X32" s="25">
         <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="33" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C33" s="79" t="s">
+      <c r="C33" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="58" t="s">
+      <c r="D33" s="71"/>
+      <c r="E33" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="59"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="58" t="s">
+      <c r="F33" s="68"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="I33" s="59"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="58" t="s">
+      <c r="I33" s="68"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="66"/>
+      <c r="T33" s="67" t="s">
         <v>115</v>
       </c>
       <c r="U33" s="69"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C34" s="79">
+      <c r="C34" s="70">
         <v>1</v>
       </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="58">
+      <c r="D34" s="71"/>
+      <c r="E34" s="67">
         <v>1</v>
       </c>
-      <c r="F34" s="59"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="58">
+      <c r="F34" s="68"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="67">
         <v>1</v>
       </c>
-      <c r="I34" s="59"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="58">
+      <c r="I34" s="68"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="67">
         <v>1</v>
       </c>
-      <c r="L34" s="59"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="60"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="58">
+      <c r="L34" s="68"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="67">
         <v>95</v>
       </c>
       <c r="U34" s="69"/>
     </row>
     <row r="35" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C35" s="79">
+      <c r="C35" s="70">
         <v>2</v>
       </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="58">
+      <c r="D35" s="71"/>
+      <c r="E35" s="67">
         <v>1</v>
       </c>
-      <c r="F35" s="59"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="58">
+      <c r="F35" s="68"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="67">
         <v>1</v>
       </c>
-      <c r="I35" s="59"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="58">
+      <c r="I35" s="68"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="67">
         <v>2</v>
       </c>
-      <c r="L35" s="59"/>
-      <c r="M35" s="60"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="60"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="60"/>
-      <c r="T35" s="58">
+      <c r="L35" s="68"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="67"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="67"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="67"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="67">
         <v>5</v>
       </c>
       <c r="U35" s="69"/>
@@ -3844,305 +3835,399 @@
       </c>
     </row>
     <row r="36" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C36" s="79">
+      <c r="C36" s="70">
         <v>3</v>
       </c>
-      <c r="D36" s="48"/>
-      <c r="E36" s="58">
+      <c r="D36" s="71"/>
+      <c r="E36" s="67">
         <v>3</v>
       </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="58">
+      <c r="F36" s="68"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="67">
         <v>1</v>
       </c>
-      <c r="I36" s="59"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="58">
+      <c r="I36" s="68"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="66"/>
+      <c r="N36" s="67">
         <v>11</v>
       </c>
-      <c r="O36" s="60"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="60"/>
-      <c r="T36" s="58">
+      <c r="O36" s="66"/>
+      <c r="P36" s="67"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="67"/>
+      <c r="S36" s="66"/>
+      <c r="T36" s="67">
         <v>100</v>
       </c>
       <c r="U36" s="69"/>
     </row>
     <row r="37" spans="3:24" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="C37" s="80">
+      <c r="C37" s="75">
         <v>4</v>
       </c>
-      <c r="D37" s="81"/>
-      <c r="E37" s="73">
+      <c r="D37" s="76"/>
+      <c r="E37" s="61">
         <v>1</v>
       </c>
-      <c r="F37" s="74"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="73">
+      <c r="F37" s="62"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="61">
         <v>45</v>
       </c>
-      <c r="I37" s="74"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="73">
+      <c r="I37" s="62"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="61">
         <v>2</v>
       </c>
-      <c r="L37" s="74"/>
-      <c r="M37" s="75"/>
-      <c r="N37" s="73"/>
-      <c r="O37" s="75"/>
-      <c r="P37" s="73"/>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="73"/>
-      <c r="S37" s="75"/>
-      <c r="T37" s="73">
+      <c r="L37" s="62"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="61"/>
+      <c r="Q37" s="63"/>
+      <c r="R37" s="61"/>
+      <c r="S37" s="63"/>
+      <c r="T37" s="61">
         <v>100</v>
       </c>
-      <c r="U37" s="76"/>
+      <c r="U37" s="64"/>
       <c r="X37" s="25" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="39" spans="3:24" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7"/>
     <row r="40" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-      <c r="I40" s="65"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="62"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="62"/>
-      <c r="O40" s="62"/>
-      <c r="P40" s="62"/>
-      <c r="Q40" s="62"/>
-      <c r="R40" s="62"/>
-      <c r="S40" s="62"/>
-      <c r="T40" s="62"/>
-      <c r="U40" s="62"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
     </row>
     <row r="41" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C41" s="67"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="62"/>
-      <c r="M41" s="62"/>
-      <c r="N41" s="62"/>
-      <c r="O41" s="62"/>
-      <c r="P41" s="62"/>
-      <c r="Q41" s="62"/>
-      <c r="R41" s="62"/>
-      <c r="S41" s="62"/>
-      <c r="T41" s="62"/>
-      <c r="U41" s="62"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
     </row>
     <row r="42" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C42" s="79" t="s">
+      <c r="C42" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="47" t="s">
+      <c r="D42" s="71"/>
+      <c r="E42" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F42" s="77"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="47" t="s">
+      <c r="F42" s="73"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="I42" s="77"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="63"/>
-      <c r="P42" s="63"/>
-      <c r="Q42" s="63"/>
-      <c r="R42" s="63"/>
-      <c r="S42" s="63"/>
-      <c r="T42" s="63"/>
-      <c r="U42" s="63"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
     </row>
     <row r="43" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="60"/>
-      <c r="E43" s="58" t="s">
+      <c r="D43" s="66"/>
+      <c r="E43" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="59"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="59"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="68"/>
       <c r="J43" s="69"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="63"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="63"/>
-      <c r="Q43" s="63"/>
-      <c r="R43" s="63"/>
-      <c r="S43" s="63"/>
-      <c r="T43" s="63"/>
-      <c r="U43" s="63"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="28"/>
+      <c r="P43" s="28"/>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="28"/>
+      <c r="T43" s="28"/>
+      <c r="U43" s="28"/>
     </row>
     <row r="44" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="D44" s="60"/>
-      <c r="E44" s="58" t="s">
+      <c r="D44" s="66"/>
+      <c r="E44" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="59"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="59"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="68"/>
       <c r="J44" s="69"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="63"/>
-      <c r="M44" s="63"/>
-      <c r="N44" s="63"/>
-      <c r="O44" s="63"/>
-      <c r="P44" s="63"/>
-      <c r="Q44" s="63"/>
-      <c r="R44" s="63"/>
-      <c r="S44" s="63"/>
-      <c r="T44" s="63"/>
-      <c r="U44" s="63"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="P44" s="28"/>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="28"/>
+      <c r="U44" s="28"/>
     </row>
     <row r="45" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="60"/>
-      <c r="E45" s="58" t="s">
+      <c r="D45" s="66"/>
+      <c r="E45" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="59"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="58" t="s">
+      <c r="F45" s="68"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="I45" s="59"/>
+      <c r="I45" s="68"/>
       <c r="J45" s="69"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="63"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="63"/>
-      <c r="R45" s="63"/>
-      <c r="S45" s="63"/>
-      <c r="T45" s="63"/>
-      <c r="U45" s="63"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="T45" s="28"/>
+      <c r="U45" s="28"/>
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C46" s="70"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="59"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="68"/>
       <c r="J46" s="69"/>
-      <c r="K46" s="63"/>
-      <c r="L46" s="63"/>
-      <c r="M46" s="63"/>
-      <c r="N46" s="63"/>
-      <c r="O46" s="63"/>
-      <c r="P46" s="63"/>
-      <c r="Q46" s="63"/>
-      <c r="R46" s="63"/>
-      <c r="S46" s="63"/>
-      <c r="T46" s="63"/>
-      <c r="U46" s="63"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="28"/>
+      <c r="R46" s="28"/>
+      <c r="S46" s="28"/>
+      <c r="T46" s="28"/>
+      <c r="U46" s="28"/>
     </row>
     <row r="47" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C47" s="70"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="59"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="68"/>
       <c r="J47" s="69"/>
-      <c r="K47" s="63"/>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="63"/>
-      <c r="P47" s="63"/>
-      <c r="Q47" s="63"/>
-      <c r="R47" s="63"/>
-      <c r="S47" s="63"/>
-      <c r="T47" s="63"/>
-      <c r="U47" s="63"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="28"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="28"/>
+      <c r="R47" s="28"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="28"/>
+      <c r="U47" s="28"/>
     </row>
     <row r="48" spans="3:24" x14ac:dyDescent="0.65">
-      <c r="C48" s="70"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="59"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="68"/>
       <c r="J48" s="69"/>
-      <c r="K48" s="63"/>
-      <c r="L48" s="63"/>
-      <c r="M48" s="63"/>
-      <c r="N48" s="63"/>
-      <c r="O48" s="63"/>
-      <c r="P48" s="63"/>
-      <c r="Q48" s="63"/>
-      <c r="R48" s="63"/>
-      <c r="S48" s="63"/>
-      <c r="T48" s="63"/>
-      <c r="U48" s="63"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="28"/>
+      <c r="P48" s="28"/>
+      <c r="Q48" s="28"/>
+      <c r="R48" s="28"/>
+      <c r="S48" s="28"/>
+      <c r="T48" s="28"/>
+      <c r="U48" s="28"/>
     </row>
     <row r="49" spans="3:21" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="C49" s="71"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="73"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="73"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="76"/>
-      <c r="K49" s="63"/>
-      <c r="L49" s="63"/>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-      <c r="O49" s="63"/>
-      <c r="P49" s="63"/>
-      <c r="Q49" s="63"/>
-      <c r="R49" s="63"/>
-      <c r="S49" s="63"/>
-      <c r="T49" s="63"/>
-      <c r="U49" s="63"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="64"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="28"/>
+      <c r="O49" s="28"/>
+      <c r="P49" s="28"/>
+      <c r="Q49" s="28"/>
+      <c r="R49" s="28"/>
+      <c r="S49" s="28"/>
+      <c r="T49" s="28"/>
+      <c r="U49" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="118">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C28:U29"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:O36"/>
     <mergeCell ref="C40:J41"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
@@ -4167,100 +4252,6 @@
     <mergeCell ref="H43:J43"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="R35:S35"/>
-    <mergeCell ref="T35:U35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C28:U29"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>